<commit_message>
Add detail view for Sub Pertanyaan with comprehensive information display
</commit_message>
<xml_diff>
--- a/public/form kuesioner.xlsx
+++ b/public/form kuesioner.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laragon\www\zona_integritas\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C05971D6-CD6C-408C-9B57-4134C5D4F11B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC07126C-260D-4AA1-9FF8-B7D5354BF680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4710,97 +4710,97 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="28" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="12" borderId="6" xfId="37" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="12" borderId="2" xfId="37" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="12" borderId="6" xfId="37" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="12" borderId="2" xfId="37" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="28" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="12" borderId="6" xfId="37" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="12" borderId="2" xfId="37" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="12" borderId="6" xfId="37" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="12" borderId="2" xfId="37" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5191,14 +5191,14 @@
       <c r="A1" s="10">
         <v>1</v>
       </c>
-      <c r="B1" s="305" t="s">
+      <c r="B1" s="311" t="s">
         <v>106</v>
       </c>
-      <c r="C1" s="305"/>
-      <c r="D1" s="305"/>
-      <c r="E1" s="305"/>
-      <c r="F1" s="305"/>
-      <c r="G1" s="305"/>
+      <c r="C1" s="311"/>
+      <c r="D1" s="311"/>
+      <c r="E1" s="311"/>
+      <c r="F1" s="311"/>
+      <c r="G1" s="311"/>
       <c r="H1" s="69" t="s">
         <v>107</v>
       </c>
@@ -5228,13 +5228,13 @@
       <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="306" t="s">
+      <c r="C3" s="309" t="s">
         <v>105</v>
       </c>
-      <c r="D3" s="306"/>
-      <c r="E3" s="306"/>
-      <c r="F3" s="306"/>
-      <c r="G3" s="306"/>
+      <c r="D3" s="309"/>
+      <c r="E3" s="309"/>
+      <c r="F3" s="309"/>
+      <c r="G3" s="309"/>
       <c r="H3" s="55">
         <v>60</v>
       </c>
@@ -5283,11 +5283,11 @@
       <c r="D5" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="304" t="s">
+      <c r="E5" s="306" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="304"/>
-      <c r="G5" s="304"/>
+      <c r="F5" s="306"/>
+      <c r="G5" s="306"/>
       <c r="H5" s="53">
         <v>4</v>
       </c>
@@ -5311,11 +5311,11 @@
       <c r="D6" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="304" t="s">
+      <c r="E6" s="306" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="304"/>
-      <c r="G6" s="304"/>
+      <c r="F6" s="306"/>
+      <c r="G6" s="306"/>
       <c r="H6" s="53">
         <v>3.5</v>
       </c>
@@ -5339,11 +5339,11 @@
       <c r="D7" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="E7" s="304" t="s">
+      <c r="E7" s="306" t="s">
         <v>134</v>
       </c>
-      <c r="F7" s="304"/>
-      <c r="G7" s="304"/>
+      <c r="F7" s="306"/>
+      <c r="G7" s="306"/>
       <c r="H7" s="53">
         <v>5</v>
       </c>
@@ -5367,11 +5367,11 @@
       <c r="D8" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="E8" s="304" t="s">
+      <c r="E8" s="306" t="s">
         <v>48</v>
       </c>
-      <c r="F8" s="304"/>
-      <c r="G8" s="304"/>
+      <c r="F8" s="306"/>
+      <c r="G8" s="306"/>
       <c r="H8" s="53">
         <v>5</v>
       </c>
@@ -5395,11 +5395,11 @@
       <c r="D9" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="304" t="s">
+      <c r="E9" s="306" t="s">
         <v>49</v>
       </c>
-      <c r="F9" s="304"/>
-      <c r="G9" s="304"/>
+      <c r="F9" s="306"/>
+      <c r="G9" s="306"/>
       <c r="H9" s="53">
         <v>7.5</v>
       </c>
@@ -5423,11 +5423,11 @@
       <c r="D10" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="304" t="s">
+      <c r="E10" s="306" t="s">
         <v>51</v>
       </c>
-      <c r="F10" s="304"/>
-      <c r="G10" s="304"/>
+      <c r="F10" s="306"/>
+      <c r="G10" s="306"/>
       <c r="H10" s="53">
         <v>5</v>
       </c>
@@ -5479,11 +5479,11 @@
       <c r="D12" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="304" t="s">
+      <c r="E12" s="306" t="s">
         <v>43</v>
       </c>
-      <c r="F12" s="304"/>
-      <c r="G12" s="304"/>
+      <c r="F12" s="306"/>
+      <c r="G12" s="306"/>
       <c r="H12" s="53">
         <v>4</v>
       </c>
@@ -5507,11 +5507,11 @@
       <c r="D13" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="304" t="s">
+      <c r="E13" s="306" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="304"/>
-      <c r="G13" s="304"/>
+      <c r="F13" s="306"/>
+      <c r="G13" s="306"/>
       <c r="H13" s="53">
         <v>3.5</v>
       </c>
@@ -5535,11 +5535,11 @@
       <c r="D14" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="E14" s="304" t="s">
+      <c r="E14" s="306" t="s">
         <v>134</v>
       </c>
-      <c r="F14" s="304"/>
-      <c r="G14" s="304"/>
+      <c r="F14" s="306"/>
+      <c r="G14" s="306"/>
       <c r="H14" s="53">
         <v>5</v>
       </c>
@@ -5563,11 +5563,11 @@
       <c r="D15" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="E15" s="304" t="s">
+      <c r="E15" s="306" t="s">
         <v>48</v>
       </c>
-      <c r="F15" s="304"/>
-      <c r="G15" s="304"/>
+      <c r="F15" s="306"/>
+      <c r="G15" s="306"/>
       <c r="H15" s="53">
         <v>5</v>
       </c>
@@ -5591,11 +5591,11 @@
       <c r="D16" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="304" t="s">
+      <c r="E16" s="306" t="s">
         <v>49</v>
       </c>
-      <c r="F16" s="304"/>
-      <c r="G16" s="304"/>
+      <c r="F16" s="306"/>
+      <c r="G16" s="306"/>
       <c r="H16" s="53">
         <v>7.5</v>
       </c>
@@ -5619,11 +5619,11 @@
       <c r="D17" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="304" t="s">
+      <c r="E17" s="306" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="304"/>
-      <c r="G17" s="304"/>
+      <c r="F17" s="306"/>
+      <c r="G17" s="306"/>
       <c r="H17" s="53">
         <v>5</v>
       </c>
@@ -5642,15 +5642,15 @@
       <c r="A18">
         <v>211</v>
       </c>
-      <c r="B18" s="310" t="s">
+      <c r="B18" s="308" t="s">
         <v>127</v>
       </c>
-      <c r="C18" s="310"/>
-      <c r="D18" s="310"/>
-      <c r="E18" s="310"/>
-      <c r="F18" s="310"/>
-      <c r="G18" s="310"/>
-      <c r="H18" s="310"/>
+      <c r="C18" s="308"/>
+      <c r="D18" s="308"/>
+      <c r="E18" s="308"/>
+      <c r="F18" s="308"/>
+      <c r="G18" s="308"/>
+      <c r="H18" s="308"/>
       <c r="I18" s="39">
         <f>'Ctt Eval'!I58</f>
         <v>55.576190476190476</v>
@@ -5679,13 +5679,13 @@
       <c r="B20" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="306" t="s">
+      <c r="C20" s="309" t="s">
         <v>128</v>
       </c>
-      <c r="D20" s="306"/>
-      <c r="E20" s="306"/>
-      <c r="F20" s="306"/>
-      <c r="G20" s="306"/>
+      <c r="D20" s="309"/>
+      <c r="E20" s="309"/>
+      <c r="F20" s="309"/>
+      <c r="G20" s="309"/>
       <c r="H20" s="57">
         <v>40</v>
       </c>
@@ -5734,11 +5734,11 @@
       <c r="D22" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="E22" s="304" t="s">
+      <c r="E22" s="306" t="s">
         <v>228</v>
       </c>
-      <c r="F22" s="304"/>
-      <c r="G22" s="304"/>
+      <c r="F22" s="306"/>
+      <c r="G22" s="306"/>
       <c r="H22" s="53">
         <v>17.5</v>
       </c>
@@ -5762,11 +5762,11 @@
       <c r="D23" s="76" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="304" t="s">
+      <c r="E23" s="306" t="s">
         <v>199</v>
       </c>
-      <c r="F23" s="304"/>
-      <c r="G23" s="304"/>
+      <c r="F23" s="306"/>
+      <c r="G23" s="306"/>
       <c r="H23" s="53">
         <v>5</v>
       </c>
@@ -5822,11 +5822,11 @@
       <c r="D25" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="E25" s="304" t="s">
+      <c r="E25" s="306" t="s">
         <v>227</v>
       </c>
-      <c r="F25" s="304"/>
-      <c r="G25" s="304"/>
+      <c r="F25" s="306"/>
+      <c r="G25" s="306"/>
       <c r="H25" s="53">
         <v>17.5</v>
       </c>
@@ -5847,15 +5847,15 @@
       <c r="A26">
         <v>222</v>
       </c>
-      <c r="B26" s="311" t="s">
+      <c r="B26" s="310" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="311"/>
-      <c r="D26" s="311"/>
-      <c r="E26" s="311"/>
-      <c r="F26" s="311"/>
-      <c r="G26" s="311"/>
-      <c r="H26" s="311"/>
+      <c r="C26" s="310"/>
+      <c r="D26" s="310"/>
+      <c r="E26" s="310"/>
+      <c r="F26" s="310"/>
+      <c r="G26" s="310"/>
+      <c r="H26" s="310"/>
       <c r="I26" s="39">
         <f>I20</f>
         <v>40</v>
@@ -5887,15 +5887,15 @@
       <c r="O27" s="1"/>
     </row>
     <row r="28" spans="1:15" ht="24">
-      <c r="B28" s="308" t="s">
+      <c r="B28" s="304" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="309"/>
-      <c r="D28" s="309"/>
-      <c r="E28" s="309"/>
-      <c r="F28" s="309"/>
-      <c r="G28" s="309"/>
-      <c r="H28" s="309"/>
+      <c r="C28" s="305"/>
+      <c r="D28" s="305"/>
+      <c r="E28" s="305"/>
+      <c r="F28" s="305"/>
+      <c r="G28" s="305"/>
+      <c r="H28" s="305"/>
       <c r="I28" s="80">
         <f>'Ctt Eval'!I68</f>
         <v>95.576190476190476</v>
@@ -5933,6 +5933,17 @@
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0"/>
   <mergeCells count="25">
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
     <mergeCell ref="B28:H28"/>
     <mergeCell ref="E16:G16"/>
     <mergeCell ref="E15:G15"/>
@@ -5947,17 +5958,6 @@
     <mergeCell ref="D24:G24"/>
     <mergeCell ref="E25:G25"/>
     <mergeCell ref="B26:H26"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="E5:G5"/>
   </mergeCells>
   <pageMargins left="2.3622047244094491" right="0.9055118110236221" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="5" scale="60" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -5998,14 +5998,14 @@
       <c r="A1" s="10">
         <v>1</v>
       </c>
-      <c r="B1" s="305" t="s">
+      <c r="B1" s="311" t="s">
         <v>106</v>
       </c>
-      <c r="C1" s="305"/>
-      <c r="D1" s="305"/>
-      <c r="E1" s="305"/>
-      <c r="F1" s="305"/>
-      <c r="G1" s="305"/>
+      <c r="C1" s="311"/>
+      <c r="D1" s="311"/>
+      <c r="E1" s="311"/>
+      <c r="F1" s="311"/>
+      <c r="G1" s="311"/>
       <c r="H1" s="69" t="s">
         <v>107</v>
       </c>
@@ -6035,13 +6035,13 @@
       <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="306" t="s">
+      <c r="C3" s="309" t="s">
         <v>105</v>
       </c>
-      <c r="D3" s="306"/>
-      <c r="E3" s="306"/>
-      <c r="F3" s="306"/>
-      <c r="G3" s="306"/>
+      <c r="D3" s="309"/>
+      <c r="E3" s="309"/>
+      <c r="F3" s="309"/>
+      <c r="G3" s="309"/>
       <c r="H3" s="55">
         <v>60</v>
       </c>
@@ -6116,10 +6116,10 @@
       <c r="E6" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="F6" s="304" t="s">
+      <c r="F6" s="306" t="s">
         <v>112</v>
       </c>
-      <c r="G6" s="304"/>
+      <c r="G6" s="306"/>
       <c r="H6" s="47">
         <v>0.5</v>
       </c>
@@ -6143,10 +6143,10 @@
       <c r="E7" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="F7" s="304" t="s">
+      <c r="F7" s="306" t="s">
         <v>217</v>
       </c>
-      <c r="G7" s="304"/>
+      <c r="G7" s="306"/>
       <c r="H7" s="47">
         <v>1</v>
       </c>
@@ -6170,10 +6170,10 @@
       <c r="E8" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="F8" s="304" t="s">
+      <c r="F8" s="306" t="s">
         <v>60</v>
       </c>
-      <c r="G8" s="304"/>
+      <c r="G8" s="306"/>
       <c r="H8" s="47">
         <v>1</v>
       </c>
@@ -6197,10 +6197,10 @@
       <c r="E9" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="F9" s="304" t="s">
+      <c r="F9" s="306" t="s">
         <v>218</v>
       </c>
-      <c r="G9" s="304"/>
+      <c r="G9" s="306"/>
       <c r="H9" s="47">
         <v>1.5</v>
       </c>
@@ -6251,10 +6251,10 @@
       <c r="E11" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="F11" s="304" t="s">
+      <c r="F11" s="306" t="s">
         <v>212</v>
       </c>
-      <c r="G11" s="304"/>
+      <c r="G11" s="306"/>
       <c r="H11" s="47">
         <v>1</v>
       </c>
@@ -6278,10 +6278,10 @@
       <c r="E12" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="F12" s="304" t="s">
+      <c r="F12" s="306" t="s">
         <v>216</v>
       </c>
-      <c r="G12" s="304"/>
+      <c r="G12" s="306"/>
       <c r="H12" s="47">
         <v>2</v>
       </c>
@@ -6305,10 +6305,10 @@
       <c r="E13" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="F13" s="304" t="s">
+      <c r="F13" s="306" t="s">
         <v>62</v>
       </c>
-      <c r="G13" s="304"/>
+      <c r="G13" s="306"/>
       <c r="H13" s="47">
         <v>0.5</v>
       </c>
@@ -6359,10 +6359,10 @@
       <c r="E15" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="F15" s="304" t="s">
+      <c r="F15" s="306" t="s">
         <v>219</v>
       </c>
-      <c r="G15" s="304"/>
+      <c r="G15" s="306"/>
       <c r="H15" s="47">
         <v>0.25</v>
       </c>
@@ -6386,10 +6386,10 @@
       <c r="E16" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="F16" s="304" t="s">
+      <c r="F16" s="306" t="s">
         <v>63</v>
       </c>
-      <c r="G16" s="304"/>
+      <c r="G16" s="306"/>
       <c r="H16" s="47">
         <v>0.5</v>
       </c>
@@ -6413,10 +6413,10 @@
       <c r="E17" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="F17" s="304" t="s">
+      <c r="F17" s="306" t="s">
         <v>220</v>
       </c>
-      <c r="G17" s="304"/>
+      <c r="G17" s="306"/>
       <c r="H17" s="47">
         <v>1.25</v>
       </c>
@@ -6440,10 +6440,10 @@
       <c r="E18" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="F18" s="304" t="s">
+      <c r="F18" s="306" t="s">
         <v>221</v>
       </c>
-      <c r="G18" s="304"/>
+      <c r="G18" s="306"/>
       <c r="H18" s="47">
         <v>2</v>
       </c>
@@ -6467,10 +6467,10 @@
       <c r="E19" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="F19" s="304" t="s">
+      <c r="F19" s="306" t="s">
         <v>222</v>
       </c>
-      <c r="G19" s="304"/>
+      <c r="G19" s="306"/>
       <c r="H19" s="47">
         <v>0.75</v>
       </c>
@@ -6494,10 +6494,10 @@
       <c r="E20" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="F20" s="304" t="s">
+      <c r="F20" s="306" t="s">
         <v>64</v>
       </c>
-      <c r="G20" s="304"/>
+      <c r="G20" s="306"/>
       <c r="H20" s="47">
         <v>0.25</v>
       </c>
@@ -6548,10 +6548,10 @@
       <c r="E22" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="F22" s="304" t="s">
+      <c r="F22" s="306" t="s">
         <v>223</v>
       </c>
-      <c r="G22" s="304"/>
+      <c r="G22" s="306"/>
       <c r="H22" s="47">
         <v>2.5</v>
       </c>
@@ -6575,10 +6575,10 @@
       <c r="E23" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="F23" s="304" t="s">
+      <c r="F23" s="306" t="s">
         <v>65</v>
       </c>
-      <c r="G23" s="304"/>
+      <c r="G23" s="306"/>
       <c r="H23" s="47">
         <v>2.5</v>
       </c>
@@ -6629,10 +6629,10 @@
       <c r="E25" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="F25" s="304" t="s">
+      <c r="F25" s="306" t="s">
         <v>66</v>
       </c>
-      <c r="G25" s="304"/>
+      <c r="G25" s="306"/>
       <c r="H25" s="47">
         <v>1.5</v>
       </c>
@@ -6656,10 +6656,10 @@
       <c r="E26" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="F26" s="304" t="s">
+      <c r="F26" s="306" t="s">
         <v>270</v>
       </c>
-      <c r="G26" s="304"/>
+      <c r="G26" s="306"/>
       <c r="H26" s="47">
         <v>1.5</v>
       </c>
@@ -6683,10 +6683,10 @@
       <c r="E27" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="F27" s="304" t="s">
+      <c r="F27" s="306" t="s">
         <v>67</v>
       </c>
-      <c r="G27" s="304"/>
+      <c r="G27" s="306"/>
       <c r="H27" s="47">
         <v>1.5</v>
       </c>
@@ -6713,7 +6713,7 @@
       <c r="F28" s="313" t="s">
         <v>68</v>
       </c>
-      <c r="G28" s="304"/>
+      <c r="G28" s="306"/>
       <c r="H28" s="47">
         <v>1.5</v>
       </c>
@@ -6737,10 +6737,10 @@
       <c r="E29" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="F29" s="304" t="s">
+      <c r="F29" s="306" t="s">
         <v>69</v>
       </c>
-      <c r="G29" s="304"/>
+      <c r="G29" s="306"/>
       <c r="H29" s="47">
         <v>1.5</v>
       </c>
@@ -6791,10 +6791,10 @@
       <c r="E31" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="F31" s="304" t="s">
+      <c r="F31" s="306" t="s">
         <v>70</v>
       </c>
-      <c r="G31" s="304"/>
+      <c r="G31" s="306"/>
       <c r="H31" s="47">
         <v>1.5</v>
       </c>
@@ -6818,10 +6818,10 @@
       <c r="E32" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="F32" s="304" t="s">
+      <c r="F32" s="306" t="s">
         <v>71</v>
       </c>
-      <c r="G32" s="304"/>
+      <c r="G32" s="306"/>
       <c r="H32" s="47">
         <v>2</v>
       </c>
@@ -6845,10 +6845,10 @@
       <c r="E33" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="F33" s="304" t="s">
+      <c r="F33" s="306" t="s">
         <v>224</v>
       </c>
-      <c r="G33" s="304"/>
+      <c r="G33" s="306"/>
       <c r="H33" s="47">
         <v>1.5</v>
       </c>
@@ -6926,10 +6926,10 @@
       <c r="E36" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="F36" s="304" t="s">
+      <c r="F36" s="306" t="s">
         <v>225</v>
       </c>
-      <c r="G36" s="304"/>
+      <c r="G36" s="306"/>
       <c r="H36" s="47">
         <v>2</v>
       </c>
@@ -6953,10 +6953,10 @@
       <c r="E37" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="F37" s="304" t="s">
+      <c r="F37" s="306" t="s">
         <v>77</v>
       </c>
-      <c r="G37" s="304" t="s">
+      <c r="G37" s="306" t="s">
         <v>77</v>
       </c>
       <c r="H37" s="47">
@@ -6982,10 +6982,10 @@
       <c r="E38" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="F38" s="304" t="s">
+      <c r="F38" s="306" t="s">
         <v>79</v>
       </c>
-      <c r="G38" s="304" t="s">
+      <c r="G38" s="306" t="s">
         <v>79</v>
       </c>
       <c r="H38" s="47">
@@ -7038,10 +7038,10 @@
       <c r="E40" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="F40" s="304" t="s">
+      <c r="F40" s="306" t="s">
         <v>83</v>
       </c>
-      <c r="G40" s="304"/>
+      <c r="G40" s="306"/>
       <c r="H40" s="47">
         <v>0.5</v>
       </c>
@@ -7065,10 +7065,10 @@
       <c r="E41" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="F41" s="304" t="s">
+      <c r="F41" s="306" t="s">
         <v>84</v>
       </c>
-      <c r="G41" s="304"/>
+      <c r="G41" s="306"/>
       <c r="H41" s="47">
         <v>1</v>
       </c>
@@ -7092,10 +7092,10 @@
       <c r="E42" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="F42" s="304" t="s">
+      <c r="F42" s="306" t="s">
         <v>89</v>
       </c>
-      <c r="G42" s="304"/>
+      <c r="G42" s="306"/>
       <c r="H42" s="47">
         <v>2</v>
       </c>
@@ -7146,10 +7146,10 @@
       <c r="E44" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="F44" s="304" t="s">
+      <c r="F44" s="306" t="s">
         <v>93</v>
       </c>
-      <c r="G44" s="304"/>
+      <c r="G44" s="306"/>
       <c r="H44" s="47">
         <v>1.5</v>
       </c>
@@ -7173,10 +7173,10 @@
       <c r="E45" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="F45" s="304" t="s">
+      <c r="F45" s="306" t="s">
         <v>138</v>
       </c>
-      <c r="G45" s="304"/>
+      <c r="G45" s="306"/>
       <c r="H45" s="47">
         <v>1.5</v>
       </c>
@@ -7200,10 +7200,10 @@
       <c r="E46" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="F46" s="304" t="s">
+      <c r="F46" s="306" t="s">
         <v>94</v>
       </c>
-      <c r="G46" s="304"/>
+      <c r="G46" s="306"/>
       <c r="H46" s="47">
         <v>2</v>
       </c>
@@ -7254,10 +7254,10 @@
       <c r="E48" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="F48" s="304" t="s">
+      <c r="F48" s="306" t="s">
         <v>136</v>
       </c>
-      <c r="G48" s="304"/>
+      <c r="G48" s="306"/>
       <c r="H48" s="47">
         <v>1</v>
       </c>
@@ -7281,10 +7281,10 @@
       <c r="E49" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="F49" s="304" t="s">
+      <c r="F49" s="306" t="s">
         <v>226</v>
       </c>
-      <c r="G49" s="304"/>
+      <c r="G49" s="306"/>
       <c r="H49" s="47">
         <v>1</v>
       </c>
@@ -7308,10 +7308,10 @@
       <c r="E50" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="F50" s="304" t="s">
+      <c r="F50" s="306" t="s">
         <v>97</v>
       </c>
-      <c r="G50" s="304"/>
+      <c r="G50" s="306"/>
       <c r="H50" s="47">
         <v>1</v>
       </c>
@@ -7362,10 +7362,10 @@
       <c r="E52" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="F52" s="304" t="s">
+      <c r="F52" s="306" t="s">
         <v>50</v>
       </c>
-      <c r="G52" s="304"/>
+      <c r="G52" s="306"/>
       <c r="H52" s="47">
         <v>2.5</v>
       </c>
@@ -7389,10 +7389,10 @@
       <c r="E53" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="F53" s="304" t="s">
+      <c r="F53" s="306" t="s">
         <v>98</v>
       </c>
-      <c r="G53" s="304"/>
+      <c r="G53" s="306"/>
       <c r="H53" s="47">
         <v>2.5</v>
       </c>
@@ -7416,10 +7416,10 @@
       <c r="E54" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="F54" s="304" t="s">
+      <c r="F54" s="306" t="s">
         <v>28</v>
       </c>
-      <c r="G54" s="304"/>
+      <c r="G54" s="306"/>
       <c r="H54" s="47">
         <v>2.5</v>
       </c>
@@ -7470,10 +7470,10 @@
       <c r="E56" s="48" t="s">
         <v>111</v>
       </c>
-      <c r="F56" s="304" t="s">
+      <c r="F56" s="306" t="s">
         <v>102</v>
       </c>
-      <c r="G56" s="304"/>
+      <c r="G56" s="306"/>
       <c r="H56" s="47">
         <v>2.5</v>
       </c>
@@ -7497,10 +7497,10 @@
       <c r="E57" s="48" t="s">
         <v>115</v>
       </c>
-      <c r="F57" s="304" t="s">
+      <c r="F57" s="306" t="s">
         <v>103</v>
       </c>
-      <c r="G57" s="304"/>
+      <c r="G57" s="306"/>
       <c r="H57" s="47">
         <v>2.5</v>
       </c>
@@ -7518,15 +7518,15 @@
       <c r="A58">
         <v>211</v>
       </c>
-      <c r="B58" s="310" t="s">
+      <c r="B58" s="308" t="s">
         <v>127</v>
       </c>
-      <c r="C58" s="310"/>
-      <c r="D58" s="310"/>
-      <c r="E58" s="310"/>
-      <c r="F58" s="310"/>
-      <c r="G58" s="310"/>
-      <c r="H58" s="310"/>
+      <c r="C58" s="308"/>
+      <c r="D58" s="308"/>
+      <c r="E58" s="308"/>
+      <c r="F58" s="308"/>
+      <c r="G58" s="308"/>
+      <c r="H58" s="308"/>
       <c r="I58" s="39">
         <f>'LKE ZI'!L198</f>
         <v>55.576190476190476</v>
@@ -7553,13 +7553,13 @@
       <c r="B60" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C60" s="306" t="s">
+      <c r="C60" s="309" t="s">
         <v>128</v>
       </c>
-      <c r="D60" s="306"/>
-      <c r="E60" s="306"/>
-      <c r="F60" s="306"/>
-      <c r="G60" s="306"/>
+      <c r="D60" s="309"/>
+      <c r="E60" s="309"/>
+      <c r="F60" s="309"/>
+      <c r="G60" s="309"/>
       <c r="H60" s="57">
         <v>40</v>
       </c>
@@ -7604,11 +7604,11 @@
       <c r="D62" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="E62" s="304" t="s">
+      <c r="E62" s="306" t="s">
         <v>228</v>
       </c>
-      <c r="F62" s="304"/>
-      <c r="G62" s="304"/>
+      <c r="F62" s="306"/>
+      <c r="G62" s="306"/>
       <c r="H62" s="53">
         <v>17.5</v>
       </c>
@@ -7629,11 +7629,11 @@
       <c r="D63" s="76" t="s">
         <v>42</v>
       </c>
-      <c r="E63" s="304" t="s">
+      <c r="E63" s="306" t="s">
         <v>199</v>
       </c>
-      <c r="F63" s="304"/>
-      <c r="G63" s="304"/>
+      <c r="F63" s="306"/>
+      <c r="G63" s="306"/>
       <c r="H63" s="53">
         <v>5</v>
       </c>
@@ -7687,11 +7687,11 @@
       <c r="D65" s="76" t="s">
         <v>120</v>
       </c>
-      <c r="E65" s="304" t="s">
+      <c r="E65" s="306" t="s">
         <v>227</v>
       </c>
-      <c r="F65" s="304"/>
-      <c r="G65" s="304"/>
+      <c r="F65" s="306"/>
+      <c r="G65" s="306"/>
       <c r="H65" s="53">
         <v>17.5</v>
       </c>
@@ -7712,15 +7712,15 @@
       <c r="A66">
         <v>221</v>
       </c>
-      <c r="B66" s="311" t="s">
+      <c r="B66" s="310" t="s">
         <v>23</v>
       </c>
-      <c r="C66" s="311"/>
-      <c r="D66" s="311"/>
-      <c r="E66" s="311"/>
-      <c r="F66" s="311"/>
-      <c r="G66" s="311"/>
-      <c r="H66" s="311"/>
+      <c r="C66" s="310"/>
+      <c r="D66" s="310"/>
+      <c r="E66" s="310"/>
+      <c r="F66" s="310"/>
+      <c r="G66" s="310"/>
+      <c r="H66" s="310"/>
       <c r="I66" s="39">
         <f>'LKE ZI'!L206</f>
         <v>40</v>
@@ -7746,15 +7746,15 @@
       <c r="A68">
         <v>223</v>
       </c>
-      <c r="B68" s="308" t="s">
+      <c r="B68" s="304" t="s">
         <v>24</v>
       </c>
-      <c r="C68" s="309"/>
-      <c r="D68" s="309"/>
-      <c r="E68" s="309"/>
-      <c r="F68" s="309"/>
-      <c r="G68" s="309"/>
-      <c r="H68" s="309"/>
+      <c r="C68" s="305"/>
+      <c r="D68" s="305"/>
+      <c r="E68" s="305"/>
+      <c r="F68" s="305"/>
+      <c r="G68" s="305"/>
+      <c r="H68" s="305"/>
       <c r="I68" s="11">
         <f>'LKE ZI'!L208</f>
         <v>95.576190476190476</v>
@@ -7804,32 +7804,33 @@
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0"/>
   <mergeCells count="65">
-    <mergeCell ref="B66:H66"/>
-    <mergeCell ref="B68:H68"/>
-    <mergeCell ref="D64:G64"/>
-    <mergeCell ref="E62:G62"/>
-    <mergeCell ref="E63:G63"/>
-    <mergeCell ref="E65:G65"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="B58:H58"/>
-    <mergeCell ref="C60:G60"/>
-    <mergeCell ref="D61:G61"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="F56:G56"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="F25:G25"/>
     <mergeCell ref="F40:G40"/>
     <mergeCell ref="F29:G29"/>
     <mergeCell ref="E30:G30"/>
@@ -7842,33 +7843,32 @@
     <mergeCell ref="F37:G37"/>
     <mergeCell ref="F38:G38"/>
     <mergeCell ref="E39:G39"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="B58:H58"/>
+    <mergeCell ref="C60:G60"/>
+    <mergeCell ref="D61:G61"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="B66:H66"/>
+    <mergeCell ref="B68:H68"/>
+    <mergeCell ref="D64:G64"/>
+    <mergeCell ref="E62:G62"/>
+    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="E65:G65"/>
   </mergeCells>
   <pageMargins left="2.3622047244094491" right="0.9055118110236221" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="5" scale="60" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -7882,8 +7882,8 @@
   </sheetPr>
   <dimension ref="A1:Q222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="B169" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection activeCell="G172" sqref="G172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75"/>
@@ -7931,14 +7931,14 @@
       <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2" s="315" t="s">
+      <c r="B2" s="333" t="s">
         <v>106</v>
       </c>
-      <c r="C2" s="315"/>
-      <c r="D2" s="315"/>
-      <c r="E2" s="315"/>
-      <c r="F2" s="315"/>
-      <c r="G2" s="315"/>
+      <c r="C2" s="333"/>
+      <c r="D2" s="333"/>
+      <c r="E2" s="333"/>
+      <c r="F2" s="333"/>
+      <c r="G2" s="333"/>
       <c r="H2" s="113" t="s">
         <v>107</v>
       </c>
@@ -7990,13 +7990,13 @@
       <c r="B4" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="316" t="s">
+      <c r="C4" s="334" t="s">
         <v>105</v>
       </c>
-      <c r="D4" s="316"/>
-      <c r="E4" s="316"/>
-      <c r="F4" s="316"/>
-      <c r="G4" s="316"/>
+      <c r="D4" s="334"/>
+      <c r="E4" s="334"/>
+      <c r="F4" s="334"/>
+      <c r="G4" s="334"/>
       <c r="H4" s="84">
         <v>60</v>
       </c>
@@ -8022,12 +8022,12 @@
       <c r="C5" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="317" t="s">
+      <c r="D5" s="331" t="s">
         <v>110</v>
       </c>
-      <c r="E5" s="317"/>
-      <c r="F5" s="317"/>
-      <c r="G5" s="317"/>
+      <c r="E5" s="331"/>
+      <c r="F5" s="331"/>
+      <c r="G5" s="331"/>
       <c r="H5" s="90">
         <v>30</v>
       </c>
@@ -8054,11 +8054,11 @@
       <c r="D6" s="96" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="314" t="s">
+      <c r="E6" s="330" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="314"/>
-      <c r="G6" s="314"/>
+      <c r="F6" s="330"/>
+      <c r="G6" s="330"/>
       <c r="H6" s="97">
         <v>4</v>
       </c>
@@ -8086,10 +8086,10 @@
       <c r="E7" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="F7" s="314" t="s">
+      <c r="F7" s="330" t="s">
         <v>331</v>
       </c>
-      <c r="G7" s="314"/>
+      <c r="G7" s="330"/>
       <c r="H7" s="103">
         <v>0.5</v>
       </c>
@@ -8195,10 +8195,10 @@
       <c r="E10" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="F10" s="314" t="s">
+      <c r="F10" s="330" t="s">
         <v>59</v>
       </c>
-      <c r="G10" s="314"/>
+      <c r="G10" s="330"/>
       <c r="H10" s="103">
         <v>1</v>
       </c>
@@ -8343,10 +8343,10 @@
       <c r="E14" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="F14" s="314" t="s">
+      <c r="F14" s="330" t="s">
         <v>60</v>
       </c>
-      <c r="G14" s="314"/>
+      <c r="G14" s="330"/>
       <c r="H14" s="103">
         <v>1</v>
       </c>
@@ -8493,10 +8493,10 @@
       <c r="E18" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="F18" s="314" t="s">
+      <c r="F18" s="330" t="s">
         <v>61</v>
       </c>
-      <c r="G18" s="314"/>
+      <c r="G18" s="330"/>
       <c r="H18" s="103">
         <v>1.5</v>
       </c>
@@ -8679,11 +8679,11 @@
       <c r="D23" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="E23" s="314" t="s">
+      <c r="E23" s="330" t="s">
         <v>45</v>
       </c>
-      <c r="F23" s="314"/>
-      <c r="G23" s="314"/>
+      <c r="F23" s="330"/>
+      <c r="G23" s="330"/>
       <c r="H23" s="97">
         <v>3.5</v>
       </c>
@@ -8711,10 +8711,10 @@
       <c r="E24" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="F24" s="314" t="s">
+      <c r="F24" s="330" t="s">
         <v>212</v>
       </c>
-      <c r="G24" s="314"/>
+      <c r="G24" s="330"/>
       <c r="H24" s="103">
         <v>1</v>
       </c>
@@ -8861,10 +8861,10 @@
       <c r="E28" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="F28" s="314" t="s">
+      <c r="F28" s="330" t="s">
         <v>216</v>
       </c>
-      <c r="G28" s="314"/>
+      <c r="G28" s="330"/>
       <c r="H28" s="103">
         <v>2</v>
       </c>
@@ -9050,10 +9050,10 @@
       <c r="E33" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="F33" s="314" t="s">
+      <c r="F33" s="330" t="s">
         <v>62</v>
       </c>
-      <c r="G33" s="314"/>
+      <c r="G33" s="330"/>
       <c r="H33" s="103">
         <v>0.5</v>
       </c>
@@ -9159,11 +9159,11 @@
       <c r="D36" s="96" t="s">
         <v>113</v>
       </c>
-      <c r="E36" s="314" t="s">
+      <c r="E36" s="330" t="s">
         <v>134</v>
       </c>
-      <c r="F36" s="314"/>
-      <c r="G36" s="314"/>
+      <c r="F36" s="330"/>
+      <c r="G36" s="330"/>
       <c r="H36" s="97">
         <v>5</v>
       </c>
@@ -9192,10 +9192,10 @@
       <c r="E37" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="F37" s="314" t="s">
+      <c r="F37" s="330" t="s">
         <v>219</v>
       </c>
-      <c r="G37" s="314"/>
+      <c r="G37" s="330"/>
       <c r="H37" s="103">
         <v>0.25</v>
       </c>
@@ -9341,10 +9341,10 @@
       <c r="E41" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="F41" s="314" t="s">
+      <c r="F41" s="330" t="s">
         <v>63</v>
       </c>
-      <c r="G41" s="314"/>
+      <c r="G41" s="330"/>
       <c r="H41" s="103">
         <v>0.5</v>
       </c>
@@ -9492,10 +9492,10 @@
       <c r="E45" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="F45" s="314" t="s">
+      <c r="F45" s="330" t="s">
         <v>220</v>
       </c>
-      <c r="G45" s="314"/>
+      <c r="G45" s="330"/>
       <c r="H45" s="103">
         <v>1.25</v>
       </c>
@@ -9760,10 +9760,10 @@
       <c r="E52" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="F52" s="314" t="s">
+      <c r="F52" s="330" t="s">
         <v>221</v>
       </c>
-      <c r="G52" s="314"/>
+      <c r="G52" s="330"/>
       <c r="H52" s="103">
         <v>2</v>
       </c>
@@ -9952,10 +9952,10 @@
       <c r="E57" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="F57" s="314" t="s">
+      <c r="F57" s="330" t="s">
         <v>222</v>
       </c>
-      <c r="G57" s="314"/>
+      <c r="G57" s="330"/>
       <c r="H57" s="103">
         <v>0.75</v>
       </c>
@@ -10023,10 +10023,10 @@
       <c r="E59" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="F59" s="314" t="s">
+      <c r="F59" s="330" t="s">
         <v>64</v>
       </c>
-      <c r="G59" s="314"/>
+      <c r="G59" s="330"/>
       <c r="H59" s="103">
         <v>0.25</v>
       </c>
@@ -10093,11 +10093,11 @@
       <c r="D61" s="96" t="s">
         <v>114</v>
       </c>
-      <c r="E61" s="314" t="s">
+      <c r="E61" s="330" t="s">
         <v>48</v>
       </c>
-      <c r="F61" s="314"/>
-      <c r="G61" s="314"/>
+      <c r="F61" s="330"/>
+      <c r="G61" s="330"/>
       <c r="H61" s="97">
         <v>5</v>
       </c>
@@ -10126,10 +10126,10 @@
       <c r="E62" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="F62" s="314" t="s">
+      <c r="F62" s="330" t="s">
         <v>223</v>
       </c>
-      <c r="G62" s="314"/>
+      <c r="G62" s="330"/>
       <c r="H62" s="103">
         <v>2.5</v>
       </c>
@@ -10277,10 +10277,10 @@
       <c r="E66" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="F66" s="314" t="s">
+      <c r="F66" s="330" t="s">
         <v>65</v>
       </c>
-      <c r="G66" s="314"/>
+      <c r="G66" s="330"/>
       <c r="H66" s="103">
         <v>2.5</v>
       </c>
@@ -10620,11 +10620,11 @@
       <c r="D75" s="96" t="s">
         <v>17</v>
       </c>
-      <c r="E75" s="314" t="s">
+      <c r="E75" s="330" t="s">
         <v>49</v>
       </c>
-      <c r="F75" s="314"/>
-      <c r="G75" s="314"/>
+      <c r="F75" s="330"/>
+      <c r="G75" s="330"/>
       <c r="H75" s="97">
         <v>7.5</v>
       </c>
@@ -10653,10 +10653,10 @@
       <c r="E76" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="F76" s="314" t="s">
+      <c r="F76" s="330" t="s">
         <v>66</v>
       </c>
-      <c r="G76" s="314"/>
+      <c r="G76" s="330"/>
       <c r="H76" s="103">
         <v>1.5</v>
       </c>
@@ -10763,10 +10763,10 @@
       <c r="E79" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="F79" s="314" t="s">
+      <c r="F79" s="330" t="s">
         <v>270</v>
       </c>
-      <c r="G79" s="314"/>
+      <c r="G79" s="330"/>
       <c r="H79" s="103">
         <v>1.5</v>
       </c>
@@ -10953,10 +10953,10 @@
       <c r="E84" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="F84" s="314" t="s">
+      <c r="F84" s="330" t="s">
         <v>67</v>
       </c>
-      <c r="G84" s="314"/>
+      <c r="G84" s="330"/>
       <c r="H84" s="103">
         <v>1.5</v>
       </c>
@@ -11133,10 +11133,10 @@
       <c r="E89" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="F89" s="318" t="s">
+      <c r="F89" s="332" t="s">
         <v>68</v>
       </c>
-      <c r="G89" s="318"/>
+      <c r="G89" s="332"/>
       <c r="H89" s="103">
         <v>1.5</v>
       </c>
@@ -11299,10 +11299,10 @@
       <c r="E94" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="F94" s="314" t="s">
+      <c r="F94" s="330" t="s">
         <v>69</v>
       </c>
-      <c r="G94" s="314"/>
+      <c r="G94" s="330"/>
       <c r="H94" s="103">
         <v>1.5</v>
       </c>
@@ -11517,11 +11517,11 @@
       <c r="D100" s="96" t="s">
         <v>18</v>
       </c>
-      <c r="E100" s="314" t="s">
+      <c r="E100" s="330" t="s">
         <v>51</v>
       </c>
-      <c r="F100" s="314"/>
-      <c r="G100" s="314"/>
+      <c r="F100" s="330"/>
+      <c r="G100" s="330"/>
       <c r="H100" s="97">
         <v>5</v>
       </c>
@@ -11550,10 +11550,10 @@
       <c r="E101" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="F101" s="314" t="s">
+      <c r="F101" s="330" t="s">
         <v>70</v>
       </c>
-      <c r="G101" s="314"/>
+      <c r="G101" s="330"/>
       <c r="H101" s="103">
         <v>1</v>
       </c>
@@ -11730,10 +11730,10 @@
       <c r="E106" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="F106" s="314" t="s">
+      <c r="F106" s="330" t="s">
         <v>71</v>
       </c>
-      <c r="G106" s="314"/>
+      <c r="G106" s="330"/>
       <c r="H106" s="103">
         <v>1</v>
       </c>
@@ -11984,10 +11984,10 @@
       <c r="E113" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="F113" s="314" t="s">
+      <c r="F113" s="330" t="s">
         <v>316</v>
       </c>
-      <c r="G113" s="314"/>
+      <c r="G113" s="330"/>
       <c r="H113" s="103">
         <v>1</v>
       </c>
@@ -12129,10 +12129,10 @@
       <c r="E117" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="F117" s="314" t="s">
+      <c r="F117" s="330" t="s">
         <v>293</v>
       </c>
-      <c r="G117" s="314"/>
+      <c r="G117" s="330"/>
       <c r="H117" s="103">
         <v>1</v>
       </c>
@@ -12270,10 +12270,10 @@
       <c r="E121" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="F121" s="314" t="s">
+      <c r="F121" s="330" t="s">
         <v>321</v>
       </c>
-      <c r="G121" s="314"/>
+      <c r="G121" s="330"/>
       <c r="H121" s="103">
         <v>1</v>
       </c>
@@ -12407,12 +12407,12 @@
       <c r="C125" s="89" t="s">
         <v>12</v>
       </c>
-      <c r="D125" s="317" t="s">
+      <c r="D125" s="331" t="s">
         <v>75</v>
       </c>
-      <c r="E125" s="317"/>
-      <c r="F125" s="317"/>
-      <c r="G125" s="317"/>
+      <c r="E125" s="331"/>
+      <c r="F125" s="331"/>
+      <c r="G125" s="331"/>
       <c r="H125" s="90">
         <v>30</v>
       </c>
@@ -12440,11 +12440,11 @@
       <c r="D126" s="96" t="s">
         <v>14</v>
       </c>
-      <c r="E126" s="314" t="s">
+      <c r="E126" s="330" t="s">
         <v>43</v>
       </c>
-      <c r="F126" s="314"/>
-      <c r="G126" s="314"/>
+      <c r="F126" s="330"/>
+      <c r="G126" s="330"/>
       <c r="H126" s="97">
         <v>4</v>
       </c>
@@ -12473,10 +12473,10 @@
       <c r="E127" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="F127" s="314" t="s">
+      <c r="F127" s="330" t="s">
         <v>76</v>
       </c>
-      <c r="G127" s="314"/>
+      <c r="G127" s="330"/>
       <c r="H127" s="103">
         <v>2</v>
       </c>
@@ -12701,10 +12701,10 @@
       <c r="E134" s="130" t="s">
         <v>115</v>
       </c>
-      <c r="F134" s="319" t="s">
+      <c r="F134" s="325" t="s">
         <v>77</v>
       </c>
-      <c r="G134" s="319" t="s">
+      <c r="G134" s="325" t="s">
         <v>77</v>
       </c>
       <c r="H134" s="144">
@@ -12772,10 +12772,10 @@
       <c r="E136" s="130" t="s">
         <v>116</v>
       </c>
-      <c r="F136" s="319" t="s">
+      <c r="F136" s="325" t="s">
         <v>79</v>
       </c>
-      <c r="G136" s="319" t="s">
+      <c r="G136" s="325" t="s">
         <v>79</v>
       </c>
       <c r="H136" s="144">
@@ -12842,11 +12842,11 @@
       <c r="D138" s="154" t="s">
         <v>15</v>
       </c>
-      <c r="E138" s="319" t="s">
+      <c r="E138" s="325" t="s">
         <v>45</v>
       </c>
-      <c r="F138" s="319"/>
-      <c r="G138" s="319"/>
+      <c r="F138" s="325"/>
+      <c r="G138" s="325"/>
       <c r="H138" s="155">
         <v>3.5</v>
       </c>
@@ -12876,10 +12876,10 @@
       <c r="E139" s="130" t="s">
         <v>111</v>
       </c>
-      <c r="F139" s="319" t="s">
+      <c r="F139" s="325" t="s">
         <v>83</v>
       </c>
-      <c r="G139" s="319"/>
+      <c r="G139" s="325"/>
       <c r="H139" s="144">
         <v>0.5</v>
       </c>
@@ -12945,10 +12945,10 @@
       <c r="E141" s="130" t="s">
         <v>115</v>
       </c>
-      <c r="F141" s="319" t="s">
+      <c r="F141" s="325" t="s">
         <v>84</v>
       </c>
-      <c r="G141" s="319"/>
+      <c r="G141" s="325"/>
       <c r="H141" s="144">
         <v>1</v>
       </c>
@@ -13050,10 +13050,10 @@
       <c r="E144" s="130" t="s">
         <v>116</v>
       </c>
-      <c r="F144" s="319" t="s">
+      <c r="F144" s="325" t="s">
         <v>89</v>
       </c>
-      <c r="G144" s="319"/>
+      <c r="G144" s="325"/>
       <c r="H144" s="144">
         <v>2</v>
       </c>
@@ -13190,11 +13190,11 @@
       <c r="D148" s="154" t="s">
         <v>113</v>
       </c>
-      <c r="E148" s="319" t="s">
+      <c r="E148" s="325" t="s">
         <v>134</v>
       </c>
-      <c r="F148" s="319"/>
-      <c r="G148" s="319"/>
+      <c r="F148" s="325"/>
+      <c r="G148" s="325"/>
       <c r="H148" s="155">
         <v>5</v>
       </c>
@@ -13224,10 +13224,10 @@
       <c r="E149" s="130" t="s">
         <v>111</v>
       </c>
-      <c r="F149" s="319" t="s">
+      <c r="F149" s="325" t="s">
         <v>93</v>
       </c>
-      <c r="G149" s="319"/>
+      <c r="G149" s="325"/>
       <c r="H149" s="144">
         <v>1.5</v>
       </c>
@@ -13293,10 +13293,10 @@
       <c r="E151" s="130" t="s">
         <v>115</v>
       </c>
-      <c r="F151" s="319" t="s">
+      <c r="F151" s="325" t="s">
         <v>121</v>
       </c>
-      <c r="G151" s="319"/>
+      <c r="G151" s="325"/>
       <c r="H151" s="144">
         <v>1.5</v>
       </c>
@@ -13362,10 +13362,10 @@
       <c r="E153" s="130" t="s">
         <v>116</v>
       </c>
-      <c r="F153" s="319" t="s">
+      <c r="F153" s="325" t="s">
         <v>94</v>
       </c>
-      <c r="G153" s="319"/>
+      <c r="G153" s="325"/>
       <c r="H153" s="144">
         <v>2</v>
       </c>
@@ -13525,11 +13525,11 @@
       <c r="D158" s="154" t="s">
         <v>114</v>
       </c>
-      <c r="E158" s="319" t="s">
+      <c r="E158" s="325" t="s">
         <v>48</v>
       </c>
-      <c r="F158" s="319"/>
-      <c r="G158" s="319"/>
+      <c r="F158" s="325"/>
+      <c r="G158" s="325"/>
       <c r="H158" s="155">
         <v>5</v>
       </c>
@@ -13556,10 +13556,10 @@
       <c r="E159" s="130" t="s">
         <v>111</v>
       </c>
-      <c r="F159" s="319" t="s">
+      <c r="F159" s="325" t="s">
         <v>136</v>
       </c>
-      <c r="G159" s="319"/>
+      <c r="G159" s="325"/>
       <c r="H159" s="144">
         <v>2</v>
       </c>
@@ -13688,10 +13688,10 @@
       <c r="E163" s="130" t="s">
         <v>115</v>
       </c>
-      <c r="F163" s="319" t="s">
+      <c r="F163" s="325" t="s">
         <v>298</v>
       </c>
-      <c r="G163" s="319"/>
+      <c r="G163" s="325"/>
       <c r="H163" s="144">
         <v>1.5</v>
       </c>
@@ -13757,10 +13757,10 @@
       <c r="E165" s="130" t="s">
         <v>116</v>
       </c>
-      <c r="F165" s="319" t="s">
+      <c r="F165" s="325" t="s">
         <v>97</v>
       </c>
-      <c r="G165" s="319"/>
+      <c r="G165" s="325"/>
       <c r="H165" s="144">
         <v>1.5</v>
       </c>
@@ -13825,11 +13825,11 @@
       <c r="D167" s="154" t="s">
         <v>17</v>
       </c>
-      <c r="E167" s="319" t="s">
+      <c r="E167" s="325" t="s">
         <v>49</v>
       </c>
-      <c r="F167" s="319"/>
-      <c r="G167" s="319"/>
+      <c r="F167" s="325"/>
+      <c r="G167" s="325"/>
       <c r="H167" s="155">
         <v>7.5</v>
       </c>
@@ -13859,10 +13859,10 @@
       <c r="E168" s="143" t="s">
         <v>111</v>
       </c>
-      <c r="F168" s="319" t="s">
+      <c r="F168" s="325" t="s">
         <v>326</v>
       </c>
-      <c r="G168" s="319"/>
+      <c r="G168" s="325"/>
       <c r="H168" s="144">
         <v>2.5</v>
       </c>
@@ -13926,10 +13926,10 @@
       <c r="E170" s="143" t="s">
         <v>115</v>
       </c>
-      <c r="F170" s="319" t="s">
+      <c r="F170" s="325" t="s">
         <v>28</v>
       </c>
-      <c r="G170" s="319"/>
+      <c r="G170" s="325"/>
       <c r="H170" s="144">
         <v>3</v>
       </c>
@@ -14090,10 +14090,10 @@
       <c r="E175" s="143" t="s">
         <v>116</v>
       </c>
-      <c r="F175" s="319" t="s">
+      <c r="F175" s="325" t="s">
         <v>355</v>
       </c>
-      <c r="G175" s="319"/>
+      <c r="G175" s="325"/>
       <c r="H175" s="144">
         <v>2</v>
       </c>
@@ -14125,10 +14125,10 @@
       <c r="E176" s="171" t="s">
         <v>111</v>
       </c>
-      <c r="F176" s="322" t="s">
+      <c r="F176" s="328" t="s">
         <v>341</v>
       </c>
-      <c r="G176" s="323"/>
+      <c r="G176" s="329"/>
       <c r="H176" s="172">
         <v>1</v>
       </c>
@@ -14351,10 +14351,10 @@
       <c r="C183" s="171"/>
       <c r="D183" s="171"/>
       <c r="E183" s="171"/>
-      <c r="F183" s="320" t="s">
+      <c r="F183" s="326" t="s">
         <v>98</v>
       </c>
-      <c r="G183" s="321"/>
+      <c r="G183" s="327"/>
       <c r="H183" s="181">
         <v>1</v>
       </c>
@@ -14577,11 +14577,11 @@
       <c r="D190" s="154" t="s">
         <v>18</v>
       </c>
-      <c r="E190" s="319" t="s">
+      <c r="E190" s="325" t="s">
         <v>51</v>
       </c>
-      <c r="F190" s="319"/>
-      <c r="G190" s="319"/>
+      <c r="F190" s="325"/>
+      <c r="G190" s="325"/>
       <c r="H190" s="155">
         <v>5</v>
       </c>
@@ -14611,10 +14611,10 @@
       <c r="E191" s="194" t="s">
         <v>111</v>
       </c>
-      <c r="F191" s="319" t="s">
+      <c r="F191" s="325" t="s">
         <v>102</v>
       </c>
-      <c r="G191" s="319"/>
+      <c r="G191" s="325"/>
       <c r="H191" s="144">
         <v>2.5</v>
       </c>
@@ -14775,10 +14775,10 @@
       <c r="E196" s="194" t="s">
         <v>115</v>
       </c>
-      <c r="F196" s="331" t="s">
+      <c r="F196" s="316" t="s">
         <v>103</v>
       </c>
-      <c r="G196" s="332"/>
+      <c r="G196" s="317"/>
       <c r="H196" s="144">
         <v>2.5</v>
       </c>
@@ -14838,16 +14838,16 @@
       <c r="A198">
         <v>211</v>
       </c>
-      <c r="B198" s="333" t="s">
+      <c r="B198" s="318" t="s">
         <v>127</v>
       </c>
-      <c r="C198" s="333"/>
-      <c r="D198" s="333"/>
-      <c r="E198" s="333"/>
-      <c r="F198" s="333"/>
-      <c r="G198" s="333"/>
-      <c r="H198" s="333"/>
-      <c r="I198" s="333"/>
+      <c r="C198" s="318"/>
+      <c r="D198" s="318"/>
+      <c r="E198" s="318"/>
+      <c r="F198" s="318"/>
+      <c r="G198" s="318"/>
+      <c r="H198" s="318"/>
+      <c r="I198" s="318"/>
       <c r="J198" s="197"/>
       <c r="K198" s="197"/>
       <c r="L198" s="197">
@@ -14888,13 +14888,13 @@
       <c r="B200" s="207" t="s">
         <v>13</v>
       </c>
-      <c r="C200" s="334" t="s">
+      <c r="C200" s="319" t="s">
         <v>128</v>
       </c>
-      <c r="D200" s="334"/>
-      <c r="E200" s="334"/>
-      <c r="F200" s="334"/>
-      <c r="G200" s="334"/>
+      <c r="D200" s="319"/>
+      <c r="E200" s="319"/>
+      <c r="F200" s="319"/>
+      <c r="G200" s="319"/>
       <c r="H200" s="208">
         <v>40</v>
       </c>
@@ -14922,12 +14922,12 @@
       <c r="C201" s="210" t="s">
         <v>1</v>
       </c>
-      <c r="D201" s="329" t="s">
+      <c r="D201" s="314" t="s">
         <v>300</v>
       </c>
-      <c r="E201" s="329"/>
-      <c r="F201" s="329"/>
-      <c r="G201" s="329"/>
+      <c r="E201" s="314"/>
+      <c r="F201" s="314"/>
+      <c r="G201" s="314"/>
       <c r="H201" s="208">
         <v>22.5</v>
       </c>
@@ -14956,11 +14956,11 @@
       <c r="D202" s="217" t="s">
         <v>41</v>
       </c>
-      <c r="E202" s="330" t="s">
+      <c r="E202" s="315" t="s">
         <v>129</v>
       </c>
-      <c r="F202" s="330"/>
-      <c r="G202" s="330"/>
+      <c r="F202" s="315"/>
+      <c r="G202" s="315"/>
       <c r="H202" s="218">
         <v>17.5</v>
       </c>
@@ -14994,11 +14994,11 @@
       <c r="D203" s="217" t="s">
         <v>42</v>
       </c>
-      <c r="E203" s="330" t="s">
+      <c r="E203" s="315" t="s">
         <v>199</v>
       </c>
-      <c r="F203" s="330"/>
-      <c r="G203" s="330"/>
+      <c r="F203" s="315"/>
+      <c r="G203" s="315"/>
       <c r="H203" s="218">
         <v>5</v>
       </c>
@@ -15031,12 +15031,12 @@
       <c r="C204" s="210" t="s">
         <v>12</v>
       </c>
-      <c r="D204" s="329" t="s">
+      <c r="D204" s="314" t="s">
         <v>301</v>
       </c>
-      <c r="E204" s="329"/>
-      <c r="F204" s="329"/>
-      <c r="G204" s="329"/>
+      <c r="E204" s="314"/>
+      <c r="F204" s="314"/>
+      <c r="G204" s="314"/>
       <c r="H204" s="208">
         <v>17.5</v>
       </c>
@@ -15065,11 +15065,11 @@
       <c r="D205" s="226" t="s">
         <v>41</v>
       </c>
-      <c r="E205" s="325" t="s">
+      <c r="E205" s="321" t="s">
         <v>130</v>
       </c>
-      <c r="F205" s="325"/>
-      <c r="G205" s="325"/>
+      <c r="F205" s="321"/>
+      <c r="G205" s="321"/>
       <c r="H205" s="227">
         <v>17.5</v>
       </c>
@@ -15098,16 +15098,16 @@
       <c r="A206">
         <v>221</v>
       </c>
-      <c r="B206" s="326" t="s">
+      <c r="B206" s="322" t="s">
         <v>23</v>
       </c>
-      <c r="C206" s="326"/>
-      <c r="D206" s="326"/>
-      <c r="E206" s="326"/>
-      <c r="F206" s="326"/>
-      <c r="G206" s="326"/>
-      <c r="H206" s="326"/>
-      <c r="I206" s="326"/>
+      <c r="C206" s="322"/>
+      <c r="D206" s="322"/>
+      <c r="E206" s="322"/>
+      <c r="F206" s="322"/>
+      <c r="G206" s="322"/>
+      <c r="H206" s="322"/>
+      <c r="I206" s="322"/>
       <c r="J206" s="197"/>
       <c r="K206" s="197"/>
       <c r="L206" s="197">
@@ -15145,18 +15145,18 @@
       <c r="A208" s="117">
         <v>223</v>
       </c>
-      <c r="B208" s="327" t="s">
+      <c r="B208" s="323" t="s">
         <v>364</v>
       </c>
-      <c r="C208" s="327"/>
-      <c r="D208" s="327"/>
-      <c r="E208" s="327"/>
-      <c r="F208" s="327"/>
-      <c r="G208" s="327"/>
-      <c r="H208" s="327"/>
-      <c r="I208" s="327"/>
-      <c r="J208" s="327"/>
-      <c r="K208" s="327"/>
+      <c r="C208" s="323"/>
+      <c r="D208" s="323"/>
+      <c r="E208" s="323"/>
+      <c r="F208" s="323"/>
+      <c r="G208" s="323"/>
+      <c r="H208" s="323"/>
+      <c r="I208" s="323"/>
+      <c r="J208" s="323"/>
+      <c r="K208" s="323"/>
       <c r="L208" s="232">
         <f>SUM(L198,L206)</f>
         <v>95.576190476190476</v>
@@ -15248,13 +15248,13 @@
       <c r="G213" s="239"/>
       <c r="H213" s="240"/>
       <c r="I213" s="241"/>
-      <c r="J213" s="328" t="s">
+      <c r="J213" s="324" t="s">
         <v>365</v>
       </c>
-      <c r="K213" s="328"/>
-      <c r="L213" s="328"/>
-      <c r="M213" s="328"/>
-      <c r="N213" s="328"/>
+      <c r="K213" s="324"/>
+      <c r="L213" s="324"/>
+      <c r="M213" s="324"/>
+      <c r="N213" s="324"/>
       <c r="O213" s="251"/>
       <c r="P213" s="302"/>
       <c r="Q213" s="138"/>
@@ -15268,11 +15268,11 @@
       <c r="G214" s="239"/>
       <c r="H214" s="240"/>
       <c r="I214" s="241"/>
-      <c r="J214" s="328"/>
-      <c r="K214" s="328"/>
-      <c r="L214" s="328"/>
-      <c r="M214" s="328"/>
-      <c r="N214" s="328"/>
+      <c r="J214" s="324"/>
+      <c r="K214" s="324"/>
+      <c r="L214" s="324"/>
+      <c r="M214" s="324"/>
+      <c r="N214" s="324"/>
       <c r="O214" s="251"/>
       <c r="P214" s="302"/>
       <c r="Q214" s="138"/>
@@ -15286,11 +15286,11 @@
       <c r="G215" s="239"/>
       <c r="H215" s="240"/>
       <c r="I215" s="241"/>
-      <c r="J215" s="328"/>
-      <c r="K215" s="328"/>
-      <c r="L215" s="328"/>
-      <c r="M215" s="328"/>
-      <c r="N215" s="328"/>
+      <c r="J215" s="324"/>
+      <c r="K215" s="324"/>
+      <c r="L215" s="324"/>
+      <c r="M215" s="324"/>
+      <c r="N215" s="324"/>
       <c r="O215" s="251"/>
       <c r="P215" s="302"/>
       <c r="Q215" s="138"/>
@@ -15304,11 +15304,11 @@
       <c r="G216" s="239"/>
       <c r="H216" s="240"/>
       <c r="I216" s="241"/>
-      <c r="J216" s="328"/>
-      <c r="K216" s="328"/>
-      <c r="L216" s="328"/>
-      <c r="M216" s="328"/>
-      <c r="N216" s="328"/>
+      <c r="J216" s="324"/>
+      <c r="K216" s="324"/>
+      <c r="L216" s="324"/>
+      <c r="M216" s="324"/>
+      <c r="N216" s="324"/>
       <c r="O216" s="251"/>
       <c r="P216" s="302"/>
       <c r="Q216" s="244"/>
@@ -15322,11 +15322,11 @@
       <c r="G217" s="239"/>
       <c r="H217" s="240"/>
       <c r="I217" s="241"/>
-      <c r="J217" s="328"/>
-      <c r="K217" s="328"/>
-      <c r="L217" s="328"/>
-      <c r="M217" s="328"/>
-      <c r="N217" s="328"/>
+      <c r="J217" s="324"/>
+      <c r="K217" s="324"/>
+      <c r="L217" s="324"/>
+      <c r="M217" s="324"/>
+      <c r="N217" s="324"/>
       <c r="O217" s="251"/>
       <c r="P217" s="302"/>
       <c r="Q217" s="244"/>
@@ -15414,11 +15414,11 @@
       <c r="G222" s="239"/>
       <c r="H222" s="240"/>
       <c r="I222" s="241"/>
-      <c r="J222" s="324" t="s">
+      <c r="J222" s="320" t="s">
         <v>330</v>
       </c>
-      <c r="K222" s="324"/>
-      <c r="L222" s="324"/>
+      <c r="K222" s="320"/>
+      <c r="L222" s="320"/>
       <c r="M222" s="246"/>
       <c r="N222" s="244"/>
       <c r="O222" s="251"/>
@@ -15429,40 +15429,28 @@
   <sheetProtection formatColumns="0" formatRows="0" autoFilter="0"/>
   <autoFilter ref="A3:O208" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <mergeCells count="72">
-    <mergeCell ref="D201:G201"/>
-    <mergeCell ref="D204:G204"/>
-    <mergeCell ref="E202:G202"/>
-    <mergeCell ref="E203:G203"/>
-    <mergeCell ref="F196:G196"/>
-    <mergeCell ref="B198:I198"/>
-    <mergeCell ref="C200:G200"/>
-    <mergeCell ref="J222:L222"/>
-    <mergeCell ref="E205:G205"/>
-    <mergeCell ref="B206:I206"/>
-    <mergeCell ref="B208:K208"/>
-    <mergeCell ref="J213:N217"/>
-    <mergeCell ref="E167:G167"/>
-    <mergeCell ref="F191:G191"/>
-    <mergeCell ref="E190:G190"/>
-    <mergeCell ref="F159:G159"/>
-    <mergeCell ref="F163:G163"/>
-    <mergeCell ref="F165:G165"/>
-    <mergeCell ref="F168:G168"/>
-    <mergeCell ref="F170:G170"/>
-    <mergeCell ref="F183:G183"/>
-    <mergeCell ref="F176:G176"/>
-    <mergeCell ref="F175:G175"/>
-    <mergeCell ref="F144:G144"/>
-    <mergeCell ref="E148:G148"/>
-    <mergeCell ref="F149:G149"/>
-    <mergeCell ref="E158:G158"/>
-    <mergeCell ref="F151:G151"/>
-    <mergeCell ref="F153:G153"/>
-    <mergeCell ref="F134:G134"/>
-    <mergeCell ref="F136:G136"/>
-    <mergeCell ref="E138:G138"/>
-    <mergeCell ref="F139:G139"/>
-    <mergeCell ref="F141:G141"/>
+    <mergeCell ref="B1:O1"/>
+    <mergeCell ref="F94:G94"/>
+    <mergeCell ref="F106:G106"/>
+    <mergeCell ref="F117:G117"/>
+    <mergeCell ref="F127:G127"/>
+    <mergeCell ref="F101:G101"/>
+    <mergeCell ref="F113:G113"/>
+    <mergeCell ref="F121:G121"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="D5:G5"/>
     <mergeCell ref="E75:G75"/>
     <mergeCell ref="E100:G100"/>
     <mergeCell ref="D125:G125"/>
@@ -15479,28 +15467,40 @@
     <mergeCell ref="F79:G79"/>
     <mergeCell ref="F84:G84"/>
     <mergeCell ref="F89:G89"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="B1:O1"/>
-    <mergeCell ref="F94:G94"/>
-    <mergeCell ref="F106:G106"/>
-    <mergeCell ref="F117:G117"/>
-    <mergeCell ref="F127:G127"/>
-    <mergeCell ref="F101:G101"/>
-    <mergeCell ref="F113:G113"/>
-    <mergeCell ref="F121:G121"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F134:G134"/>
+    <mergeCell ref="F136:G136"/>
+    <mergeCell ref="E138:G138"/>
+    <mergeCell ref="F139:G139"/>
+    <mergeCell ref="F141:G141"/>
+    <mergeCell ref="F144:G144"/>
+    <mergeCell ref="E148:G148"/>
+    <mergeCell ref="F149:G149"/>
+    <mergeCell ref="E158:G158"/>
+    <mergeCell ref="F151:G151"/>
+    <mergeCell ref="F153:G153"/>
+    <mergeCell ref="E167:G167"/>
+    <mergeCell ref="F191:G191"/>
+    <mergeCell ref="E190:G190"/>
+    <mergeCell ref="F159:G159"/>
+    <mergeCell ref="F163:G163"/>
+    <mergeCell ref="F165:G165"/>
+    <mergeCell ref="F168:G168"/>
+    <mergeCell ref="F170:G170"/>
+    <mergeCell ref="F183:G183"/>
+    <mergeCell ref="F176:G176"/>
+    <mergeCell ref="F175:G175"/>
+    <mergeCell ref="J222:L222"/>
+    <mergeCell ref="E205:G205"/>
+    <mergeCell ref="B206:I206"/>
+    <mergeCell ref="B208:K208"/>
+    <mergeCell ref="J213:N217"/>
+    <mergeCell ref="D201:G201"/>
+    <mergeCell ref="D204:G204"/>
+    <mergeCell ref="E202:G202"/>
+    <mergeCell ref="E203:G203"/>
+    <mergeCell ref="F196:G196"/>
+    <mergeCell ref="B198:I198"/>
+    <mergeCell ref="C200:G200"/>
   </mergeCells>
   <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K150 K12:K13 K29:K32 K63:K64 K51 K74 K60 K152 K34:K35 K77 K72 K82:K83 K124 K91:K93 K98:K99 K9 K20:K21 K115:K116 K142:K143 K119 K85 K87:K88" xr:uid="{00000000-0002-0000-0200-000000000000}">

</xml_diff>

<commit_message>
refactor: rename autoSave method to submit and update related routes
</commit_message>
<xml_diff>
--- a/public/form kuesioner.xlsx
+++ b/public/form kuesioner.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laragon\www\zona_integritas\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC07126C-260D-4AA1-9FF8-B7D5354BF680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A7E4094-B496-49BC-9C89-CB3A19EF6417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4710,36 +4710,87 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="12" borderId="6" xfId="37" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="12" borderId="2" xfId="37" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="12" borderId="6" xfId="37" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="12" borderId="2" xfId="37" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -4757,57 +4808,6 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="12" borderId="6" xfId="37" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="12" borderId="2" xfId="37" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="12" borderId="6" xfId="37" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="12" borderId="2" xfId="37" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="39">
@@ -5191,14 +5191,14 @@
       <c r="A1" s="10">
         <v>1</v>
       </c>
-      <c r="B1" s="311" t="s">
+      <c r="B1" s="305" t="s">
         <v>106</v>
       </c>
-      <c r="C1" s="311"/>
-      <c r="D1" s="311"/>
-      <c r="E1" s="311"/>
-      <c r="F1" s="311"/>
-      <c r="G1" s="311"/>
+      <c r="C1" s="305"/>
+      <c r="D1" s="305"/>
+      <c r="E1" s="305"/>
+      <c r="F1" s="305"/>
+      <c r="G1" s="305"/>
       <c r="H1" s="69" t="s">
         <v>107</v>
       </c>
@@ -5228,13 +5228,13 @@
       <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="309" t="s">
+      <c r="C3" s="306" t="s">
         <v>105</v>
       </c>
-      <c r="D3" s="309"/>
-      <c r="E3" s="309"/>
-      <c r="F3" s="309"/>
-      <c r="G3" s="309"/>
+      <c r="D3" s="306"/>
+      <c r="E3" s="306"/>
+      <c r="F3" s="306"/>
+      <c r="G3" s="306"/>
       <c r="H3" s="55">
         <v>60</v>
       </c>
@@ -5283,11 +5283,11 @@
       <c r="D5" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="306" t="s">
+      <c r="E5" s="304" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="306"/>
-      <c r="G5" s="306"/>
+      <c r="F5" s="304"/>
+      <c r="G5" s="304"/>
       <c r="H5" s="53">
         <v>4</v>
       </c>
@@ -5311,11 +5311,11 @@
       <c r="D6" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="306" t="s">
+      <c r="E6" s="304" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="306"/>
-      <c r="G6" s="306"/>
+      <c r="F6" s="304"/>
+      <c r="G6" s="304"/>
       <c r="H6" s="53">
         <v>3.5</v>
       </c>
@@ -5339,11 +5339,11 @@
       <c r="D7" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="E7" s="306" t="s">
+      <c r="E7" s="304" t="s">
         <v>134</v>
       </c>
-      <c r="F7" s="306"/>
-      <c r="G7" s="306"/>
+      <c r="F7" s="304"/>
+      <c r="G7" s="304"/>
       <c r="H7" s="53">
         <v>5</v>
       </c>
@@ -5367,11 +5367,11 @@
       <c r="D8" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="E8" s="306" t="s">
+      <c r="E8" s="304" t="s">
         <v>48</v>
       </c>
-      <c r="F8" s="306"/>
-      <c r="G8" s="306"/>
+      <c r="F8" s="304"/>
+      <c r="G8" s="304"/>
       <c r="H8" s="53">
         <v>5</v>
       </c>
@@ -5395,11 +5395,11 @@
       <c r="D9" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="306" t="s">
+      <c r="E9" s="304" t="s">
         <v>49</v>
       </c>
-      <c r="F9" s="306"/>
-      <c r="G9" s="306"/>
+      <c r="F9" s="304"/>
+      <c r="G9" s="304"/>
       <c r="H9" s="53">
         <v>7.5</v>
       </c>
@@ -5423,11 +5423,11 @@
       <c r="D10" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="306" t="s">
+      <c r="E10" s="304" t="s">
         <v>51</v>
       </c>
-      <c r="F10" s="306"/>
-      <c r="G10" s="306"/>
+      <c r="F10" s="304"/>
+      <c r="G10" s="304"/>
       <c r="H10" s="53">
         <v>5</v>
       </c>
@@ -5479,11 +5479,11 @@
       <c r="D12" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="306" t="s">
+      <c r="E12" s="304" t="s">
         <v>43</v>
       </c>
-      <c r="F12" s="306"/>
-      <c r="G12" s="306"/>
+      <c r="F12" s="304"/>
+      <c r="G12" s="304"/>
       <c r="H12" s="53">
         <v>4</v>
       </c>
@@ -5507,11 +5507,11 @@
       <c r="D13" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="306" t="s">
+      <c r="E13" s="304" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="306"/>
-      <c r="G13" s="306"/>
+      <c r="F13" s="304"/>
+      <c r="G13" s="304"/>
       <c r="H13" s="53">
         <v>3.5</v>
       </c>
@@ -5535,11 +5535,11 @@
       <c r="D14" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="E14" s="306" t="s">
+      <c r="E14" s="304" t="s">
         <v>134</v>
       </c>
-      <c r="F14" s="306"/>
-      <c r="G14" s="306"/>
+      <c r="F14" s="304"/>
+      <c r="G14" s="304"/>
       <c r="H14" s="53">
         <v>5</v>
       </c>
@@ -5563,11 +5563,11 @@
       <c r="D15" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="E15" s="306" t="s">
+      <c r="E15" s="304" t="s">
         <v>48</v>
       </c>
-      <c r="F15" s="306"/>
-      <c r="G15" s="306"/>
+      <c r="F15" s="304"/>
+      <c r="G15" s="304"/>
       <c r="H15" s="53">
         <v>5</v>
       </c>
@@ -5591,11 +5591,11 @@
       <c r="D16" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="306" t="s">
+      <c r="E16" s="304" t="s">
         <v>49</v>
       </c>
-      <c r="F16" s="306"/>
-      <c r="G16" s="306"/>
+      <c r="F16" s="304"/>
+      <c r="G16" s="304"/>
       <c r="H16" s="53">
         <v>7.5</v>
       </c>
@@ -5619,11 +5619,11 @@
       <c r="D17" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="306" t="s">
+      <c r="E17" s="304" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="306"/>
-      <c r="G17" s="306"/>
+      <c r="F17" s="304"/>
+      <c r="G17" s="304"/>
       <c r="H17" s="53">
         <v>5</v>
       </c>
@@ -5642,15 +5642,15 @@
       <c r="A18">
         <v>211</v>
       </c>
-      <c r="B18" s="308" t="s">
+      <c r="B18" s="310" t="s">
         <v>127</v>
       </c>
-      <c r="C18" s="308"/>
-      <c r="D18" s="308"/>
-      <c r="E18" s="308"/>
-      <c r="F18" s="308"/>
-      <c r="G18" s="308"/>
-      <c r="H18" s="308"/>
+      <c r="C18" s="310"/>
+      <c r="D18" s="310"/>
+      <c r="E18" s="310"/>
+      <c r="F18" s="310"/>
+      <c r="G18" s="310"/>
+      <c r="H18" s="310"/>
       <c r="I18" s="39">
         <f>'Ctt Eval'!I58</f>
         <v>55.576190476190476</v>
@@ -5679,13 +5679,13 @@
       <c r="B20" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="309" t="s">
+      <c r="C20" s="306" t="s">
         <v>128</v>
       </c>
-      <c r="D20" s="309"/>
-      <c r="E20" s="309"/>
-      <c r="F20" s="309"/>
-      <c r="G20" s="309"/>
+      <c r="D20" s="306"/>
+      <c r="E20" s="306"/>
+      <c r="F20" s="306"/>
+      <c r="G20" s="306"/>
       <c r="H20" s="57">
         <v>40</v>
       </c>
@@ -5734,11 +5734,11 @@
       <c r="D22" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="E22" s="306" t="s">
+      <c r="E22" s="304" t="s">
         <v>228</v>
       </c>
-      <c r="F22" s="306"/>
-      <c r="G22" s="306"/>
+      <c r="F22" s="304"/>
+      <c r="G22" s="304"/>
       <c r="H22" s="53">
         <v>17.5</v>
       </c>
@@ -5762,11 +5762,11 @@
       <c r="D23" s="76" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="306" t="s">
+      <c r="E23" s="304" t="s">
         <v>199</v>
       </c>
-      <c r="F23" s="306"/>
-      <c r="G23" s="306"/>
+      <c r="F23" s="304"/>
+      <c r="G23" s="304"/>
       <c r="H23" s="53">
         <v>5</v>
       </c>
@@ -5822,11 +5822,11 @@
       <c r="D25" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="E25" s="306" t="s">
+      <c r="E25" s="304" t="s">
         <v>227</v>
       </c>
-      <c r="F25" s="306"/>
-      <c r="G25" s="306"/>
+      <c r="F25" s="304"/>
+      <c r="G25" s="304"/>
       <c r="H25" s="53">
         <v>17.5</v>
       </c>
@@ -5847,15 +5847,15 @@
       <c r="A26">
         <v>222</v>
       </c>
-      <c r="B26" s="310" t="s">
+      <c r="B26" s="311" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="310"/>
-      <c r="D26" s="310"/>
-      <c r="E26" s="310"/>
-      <c r="F26" s="310"/>
-      <c r="G26" s="310"/>
-      <c r="H26" s="310"/>
+      <c r="C26" s="311"/>
+      <c r="D26" s="311"/>
+      <c r="E26" s="311"/>
+      <c r="F26" s="311"/>
+      <c r="G26" s="311"/>
+      <c r="H26" s="311"/>
       <c r="I26" s="39">
         <f>I20</f>
         <v>40</v>
@@ -5887,15 +5887,15 @@
       <c r="O27" s="1"/>
     </row>
     <row r="28" spans="1:15" ht="24">
-      <c r="B28" s="304" t="s">
+      <c r="B28" s="308" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="305"/>
-      <c r="D28" s="305"/>
-      <c r="E28" s="305"/>
-      <c r="F28" s="305"/>
-      <c r="G28" s="305"/>
-      <c r="H28" s="305"/>
+      <c r="C28" s="309"/>
+      <c r="D28" s="309"/>
+      <c r="E28" s="309"/>
+      <c r="F28" s="309"/>
+      <c r="G28" s="309"/>
+      <c r="H28" s="309"/>
       <c r="I28" s="80">
         <f>'Ctt Eval'!I68</f>
         <v>95.576190476190476</v>
@@ -5933,17 +5933,6 @@
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0"/>
   <mergeCells count="25">
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
     <mergeCell ref="B28:H28"/>
     <mergeCell ref="E16:G16"/>
     <mergeCell ref="E15:G15"/>
@@ -5958,6 +5947,17 @@
     <mergeCell ref="D24:G24"/>
     <mergeCell ref="E25:G25"/>
     <mergeCell ref="B26:H26"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="E5:G5"/>
   </mergeCells>
   <pageMargins left="2.3622047244094491" right="0.9055118110236221" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="5" scale="60" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -5998,14 +5998,14 @@
       <c r="A1" s="10">
         <v>1</v>
       </c>
-      <c r="B1" s="311" t="s">
+      <c r="B1" s="305" t="s">
         <v>106</v>
       </c>
-      <c r="C1" s="311"/>
-      <c r="D1" s="311"/>
-      <c r="E1" s="311"/>
-      <c r="F1" s="311"/>
-      <c r="G1" s="311"/>
+      <c r="C1" s="305"/>
+      <c r="D1" s="305"/>
+      <c r="E1" s="305"/>
+      <c r="F1" s="305"/>
+      <c r="G1" s="305"/>
       <c r="H1" s="69" t="s">
         <v>107</v>
       </c>
@@ -6035,13 +6035,13 @@
       <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="309" t="s">
+      <c r="C3" s="306" t="s">
         <v>105</v>
       </c>
-      <c r="D3" s="309"/>
-      <c r="E3" s="309"/>
-      <c r="F3" s="309"/>
-      <c r="G3" s="309"/>
+      <c r="D3" s="306"/>
+      <c r="E3" s="306"/>
+      <c r="F3" s="306"/>
+      <c r="G3" s="306"/>
       <c r="H3" s="55">
         <v>60</v>
       </c>
@@ -6116,10 +6116,10 @@
       <c r="E6" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="F6" s="306" t="s">
+      <c r="F6" s="304" t="s">
         <v>112</v>
       </c>
-      <c r="G6" s="306"/>
+      <c r="G6" s="304"/>
       <c r="H6" s="47">
         <v>0.5</v>
       </c>
@@ -6143,10 +6143,10 @@
       <c r="E7" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="F7" s="306" t="s">
+      <c r="F7" s="304" t="s">
         <v>217</v>
       </c>
-      <c r="G7" s="306"/>
+      <c r="G7" s="304"/>
       <c r="H7" s="47">
         <v>1</v>
       </c>
@@ -6170,10 +6170,10 @@
       <c r="E8" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="F8" s="306" t="s">
+      <c r="F8" s="304" t="s">
         <v>60</v>
       </c>
-      <c r="G8" s="306"/>
+      <c r="G8" s="304"/>
       <c r="H8" s="47">
         <v>1</v>
       </c>
@@ -6197,10 +6197,10 @@
       <c r="E9" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="F9" s="306" t="s">
+      <c r="F9" s="304" t="s">
         <v>218</v>
       </c>
-      <c r="G9" s="306"/>
+      <c r="G9" s="304"/>
       <c r="H9" s="47">
         <v>1.5</v>
       </c>
@@ -6251,10 +6251,10 @@
       <c r="E11" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="F11" s="306" t="s">
+      <c r="F11" s="304" t="s">
         <v>212</v>
       </c>
-      <c r="G11" s="306"/>
+      <c r="G11" s="304"/>
       <c r="H11" s="47">
         <v>1</v>
       </c>
@@ -6278,10 +6278,10 @@
       <c r="E12" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="F12" s="306" t="s">
+      <c r="F12" s="304" t="s">
         <v>216</v>
       </c>
-      <c r="G12" s="306"/>
+      <c r="G12" s="304"/>
       <c r="H12" s="47">
         <v>2</v>
       </c>
@@ -6305,10 +6305,10 @@
       <c r="E13" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="F13" s="306" t="s">
+      <c r="F13" s="304" t="s">
         <v>62</v>
       </c>
-      <c r="G13" s="306"/>
+      <c r="G13" s="304"/>
       <c r="H13" s="47">
         <v>0.5</v>
       </c>
@@ -6359,10 +6359,10 @@
       <c r="E15" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="F15" s="306" t="s">
+      <c r="F15" s="304" t="s">
         <v>219</v>
       </c>
-      <c r="G15" s="306"/>
+      <c r="G15" s="304"/>
       <c r="H15" s="47">
         <v>0.25</v>
       </c>
@@ -6386,10 +6386,10 @@
       <c r="E16" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="F16" s="306" t="s">
+      <c r="F16" s="304" t="s">
         <v>63</v>
       </c>
-      <c r="G16" s="306"/>
+      <c r="G16" s="304"/>
       <c r="H16" s="47">
         <v>0.5</v>
       </c>
@@ -6413,10 +6413,10 @@
       <c r="E17" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="F17" s="306" t="s">
+      <c r="F17" s="304" t="s">
         <v>220</v>
       </c>
-      <c r="G17" s="306"/>
+      <c r="G17" s="304"/>
       <c r="H17" s="47">
         <v>1.25</v>
       </c>
@@ -6440,10 +6440,10 @@
       <c r="E18" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="F18" s="306" t="s">
+      <c r="F18" s="304" t="s">
         <v>221</v>
       </c>
-      <c r="G18" s="306"/>
+      <c r="G18" s="304"/>
       <c r="H18" s="47">
         <v>2</v>
       </c>
@@ -6467,10 +6467,10 @@
       <c r="E19" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="F19" s="306" t="s">
+      <c r="F19" s="304" t="s">
         <v>222</v>
       </c>
-      <c r="G19" s="306"/>
+      <c r="G19" s="304"/>
       <c r="H19" s="47">
         <v>0.75</v>
       </c>
@@ -6494,10 +6494,10 @@
       <c r="E20" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="F20" s="306" t="s">
+      <c r="F20" s="304" t="s">
         <v>64</v>
       </c>
-      <c r="G20" s="306"/>
+      <c r="G20" s="304"/>
       <c r="H20" s="47">
         <v>0.25</v>
       </c>
@@ -6548,10 +6548,10 @@
       <c r="E22" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="F22" s="306" t="s">
+      <c r="F22" s="304" t="s">
         <v>223</v>
       </c>
-      <c r="G22" s="306"/>
+      <c r="G22" s="304"/>
       <c r="H22" s="47">
         <v>2.5</v>
       </c>
@@ -6575,10 +6575,10 @@
       <c r="E23" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="F23" s="306" t="s">
+      <c r="F23" s="304" t="s">
         <v>65</v>
       </c>
-      <c r="G23" s="306"/>
+      <c r="G23" s="304"/>
       <c r="H23" s="47">
         <v>2.5</v>
       </c>
@@ -6629,10 +6629,10 @@
       <c r="E25" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="F25" s="306" t="s">
+      <c r="F25" s="304" t="s">
         <v>66</v>
       </c>
-      <c r="G25" s="306"/>
+      <c r="G25" s="304"/>
       <c r="H25" s="47">
         <v>1.5</v>
       </c>
@@ -6656,10 +6656,10 @@
       <c r="E26" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="F26" s="306" t="s">
+      <c r="F26" s="304" t="s">
         <v>270</v>
       </c>
-      <c r="G26" s="306"/>
+      <c r="G26" s="304"/>
       <c r="H26" s="47">
         <v>1.5</v>
       </c>
@@ -6683,10 +6683,10 @@
       <c r="E27" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="F27" s="306" t="s">
+      <c r="F27" s="304" t="s">
         <v>67</v>
       </c>
-      <c r="G27" s="306"/>
+      <c r="G27" s="304"/>
       <c r="H27" s="47">
         <v>1.5</v>
       </c>
@@ -6713,7 +6713,7 @@
       <c r="F28" s="313" t="s">
         <v>68</v>
       </c>
-      <c r="G28" s="306"/>
+      <c r="G28" s="304"/>
       <c r="H28" s="47">
         <v>1.5</v>
       </c>
@@ -6737,10 +6737,10 @@
       <c r="E29" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="F29" s="306" t="s">
+      <c r="F29" s="304" t="s">
         <v>69</v>
       </c>
-      <c r="G29" s="306"/>
+      <c r="G29" s="304"/>
       <c r="H29" s="47">
         <v>1.5</v>
       </c>
@@ -6791,10 +6791,10 @@
       <c r="E31" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="F31" s="306" t="s">
+      <c r="F31" s="304" t="s">
         <v>70</v>
       </c>
-      <c r="G31" s="306"/>
+      <c r="G31" s="304"/>
       <c r="H31" s="47">
         <v>1.5</v>
       </c>
@@ -6818,10 +6818,10 @@
       <c r="E32" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="F32" s="306" t="s">
+      <c r="F32" s="304" t="s">
         <v>71</v>
       </c>
-      <c r="G32" s="306"/>
+      <c r="G32" s="304"/>
       <c r="H32" s="47">
         <v>2</v>
       </c>
@@ -6845,10 +6845,10 @@
       <c r="E33" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="F33" s="306" t="s">
+      <c r="F33" s="304" t="s">
         <v>224</v>
       </c>
-      <c r="G33" s="306"/>
+      <c r="G33" s="304"/>
       <c r="H33" s="47">
         <v>1.5</v>
       </c>
@@ -6926,10 +6926,10 @@
       <c r="E36" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="F36" s="306" t="s">
+      <c r="F36" s="304" t="s">
         <v>225</v>
       </c>
-      <c r="G36" s="306"/>
+      <c r="G36" s="304"/>
       <c r="H36" s="47">
         <v>2</v>
       </c>
@@ -6953,10 +6953,10 @@
       <c r="E37" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="F37" s="306" t="s">
+      <c r="F37" s="304" t="s">
         <v>77</v>
       </c>
-      <c r="G37" s="306" t="s">
+      <c r="G37" s="304" t="s">
         <v>77</v>
       </c>
       <c r="H37" s="47">
@@ -6982,10 +6982,10 @@
       <c r="E38" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="F38" s="306" t="s">
+      <c r="F38" s="304" t="s">
         <v>79</v>
       </c>
-      <c r="G38" s="306" t="s">
+      <c r="G38" s="304" t="s">
         <v>79</v>
       </c>
       <c r="H38" s="47">
@@ -7038,10 +7038,10 @@
       <c r="E40" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="F40" s="306" t="s">
+      <c r="F40" s="304" t="s">
         <v>83</v>
       </c>
-      <c r="G40" s="306"/>
+      <c r="G40" s="304"/>
       <c r="H40" s="47">
         <v>0.5</v>
       </c>
@@ -7065,10 +7065,10 @@
       <c r="E41" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="F41" s="306" t="s">
+      <c r="F41" s="304" t="s">
         <v>84</v>
       </c>
-      <c r="G41" s="306"/>
+      <c r="G41" s="304"/>
       <c r="H41" s="47">
         <v>1</v>
       </c>
@@ -7092,10 +7092,10 @@
       <c r="E42" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="F42" s="306" t="s">
+      <c r="F42" s="304" t="s">
         <v>89</v>
       </c>
-      <c r="G42" s="306"/>
+      <c r="G42" s="304"/>
       <c r="H42" s="47">
         <v>2</v>
       </c>
@@ -7146,10 +7146,10 @@
       <c r="E44" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="F44" s="306" t="s">
+      <c r="F44" s="304" t="s">
         <v>93</v>
       </c>
-      <c r="G44" s="306"/>
+      <c r="G44" s="304"/>
       <c r="H44" s="47">
         <v>1.5</v>
       </c>
@@ -7173,10 +7173,10 @@
       <c r="E45" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="F45" s="306" t="s">
+      <c r="F45" s="304" t="s">
         <v>138</v>
       </c>
-      <c r="G45" s="306"/>
+      <c r="G45" s="304"/>
       <c r="H45" s="47">
         <v>1.5</v>
       </c>
@@ -7200,10 +7200,10 @@
       <c r="E46" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="F46" s="306" t="s">
+      <c r="F46" s="304" t="s">
         <v>94</v>
       </c>
-      <c r="G46" s="306"/>
+      <c r="G46" s="304"/>
       <c r="H46" s="47">
         <v>2</v>
       </c>
@@ -7254,10 +7254,10 @@
       <c r="E48" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="F48" s="306" t="s">
+      <c r="F48" s="304" t="s">
         <v>136</v>
       </c>
-      <c r="G48" s="306"/>
+      <c r="G48" s="304"/>
       <c r="H48" s="47">
         <v>1</v>
       </c>
@@ -7281,10 +7281,10 @@
       <c r="E49" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="F49" s="306" t="s">
+      <c r="F49" s="304" t="s">
         <v>226</v>
       </c>
-      <c r="G49" s="306"/>
+      <c r="G49" s="304"/>
       <c r="H49" s="47">
         <v>1</v>
       </c>
@@ -7308,10 +7308,10 @@
       <c r="E50" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="F50" s="306" t="s">
+      <c r="F50" s="304" t="s">
         <v>97</v>
       </c>
-      <c r="G50" s="306"/>
+      <c r="G50" s="304"/>
       <c r="H50" s="47">
         <v>1</v>
       </c>
@@ -7362,10 +7362,10 @@
       <c r="E52" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="F52" s="306" t="s">
+      <c r="F52" s="304" t="s">
         <v>50</v>
       </c>
-      <c r="G52" s="306"/>
+      <c r="G52" s="304"/>
       <c r="H52" s="47">
         <v>2.5</v>
       </c>
@@ -7389,10 +7389,10 @@
       <c r="E53" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="F53" s="306" t="s">
+      <c r="F53" s="304" t="s">
         <v>98</v>
       </c>
-      <c r="G53" s="306"/>
+      <c r="G53" s="304"/>
       <c r="H53" s="47">
         <v>2.5</v>
       </c>
@@ -7416,10 +7416,10 @@
       <c r="E54" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="F54" s="306" t="s">
+      <c r="F54" s="304" t="s">
         <v>28</v>
       </c>
-      <c r="G54" s="306"/>
+      <c r="G54" s="304"/>
       <c r="H54" s="47">
         <v>2.5</v>
       </c>
@@ -7470,10 +7470,10 @@
       <c r="E56" s="48" t="s">
         <v>111</v>
       </c>
-      <c r="F56" s="306" t="s">
+      <c r="F56" s="304" t="s">
         <v>102</v>
       </c>
-      <c r="G56" s="306"/>
+      <c r="G56" s="304"/>
       <c r="H56" s="47">
         <v>2.5</v>
       </c>
@@ -7497,10 +7497,10 @@
       <c r="E57" s="48" t="s">
         <v>115</v>
       </c>
-      <c r="F57" s="306" t="s">
+      <c r="F57" s="304" t="s">
         <v>103</v>
       </c>
-      <c r="G57" s="306"/>
+      <c r="G57" s="304"/>
       <c r="H57" s="47">
         <v>2.5</v>
       </c>
@@ -7518,15 +7518,15 @@
       <c r="A58">
         <v>211</v>
       </c>
-      <c r="B58" s="308" t="s">
+      <c r="B58" s="310" t="s">
         <v>127</v>
       </c>
-      <c r="C58" s="308"/>
-      <c r="D58" s="308"/>
-      <c r="E58" s="308"/>
-      <c r="F58" s="308"/>
-      <c r="G58" s="308"/>
-      <c r="H58" s="308"/>
+      <c r="C58" s="310"/>
+      <c r="D58" s="310"/>
+      <c r="E58" s="310"/>
+      <c r="F58" s="310"/>
+      <c r="G58" s="310"/>
+      <c r="H58" s="310"/>
       <c r="I58" s="39">
         <f>'LKE ZI'!L198</f>
         <v>55.576190476190476</v>
@@ -7553,13 +7553,13 @@
       <c r="B60" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C60" s="309" t="s">
+      <c r="C60" s="306" t="s">
         <v>128</v>
       </c>
-      <c r="D60" s="309"/>
-      <c r="E60" s="309"/>
-      <c r="F60" s="309"/>
-      <c r="G60" s="309"/>
+      <c r="D60" s="306"/>
+      <c r="E60" s="306"/>
+      <c r="F60" s="306"/>
+      <c r="G60" s="306"/>
       <c r="H60" s="57">
         <v>40</v>
       </c>
@@ -7604,11 +7604,11 @@
       <c r="D62" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="E62" s="306" t="s">
+      <c r="E62" s="304" t="s">
         <v>228</v>
       </c>
-      <c r="F62" s="306"/>
-      <c r="G62" s="306"/>
+      <c r="F62" s="304"/>
+      <c r="G62" s="304"/>
       <c r="H62" s="53">
         <v>17.5</v>
       </c>
@@ -7629,11 +7629,11 @@
       <c r="D63" s="76" t="s">
         <v>42</v>
       </c>
-      <c r="E63" s="306" t="s">
+      <c r="E63" s="304" t="s">
         <v>199</v>
       </c>
-      <c r="F63" s="306"/>
-      <c r="G63" s="306"/>
+      <c r="F63" s="304"/>
+      <c r="G63" s="304"/>
       <c r="H63" s="53">
         <v>5</v>
       </c>
@@ -7687,11 +7687,11 @@
       <c r="D65" s="76" t="s">
         <v>120</v>
       </c>
-      <c r="E65" s="306" t="s">
+      <c r="E65" s="304" t="s">
         <v>227</v>
       </c>
-      <c r="F65" s="306"/>
-      <c r="G65" s="306"/>
+      <c r="F65" s="304"/>
+      <c r="G65" s="304"/>
       <c r="H65" s="53">
         <v>17.5</v>
       </c>
@@ -7712,15 +7712,15 @@
       <c r="A66">
         <v>221</v>
       </c>
-      <c r="B66" s="310" t="s">
+      <c r="B66" s="311" t="s">
         <v>23</v>
       </c>
-      <c r="C66" s="310"/>
-      <c r="D66" s="310"/>
-      <c r="E66" s="310"/>
-      <c r="F66" s="310"/>
-      <c r="G66" s="310"/>
-      <c r="H66" s="310"/>
+      <c r="C66" s="311"/>
+      <c r="D66" s="311"/>
+      <c r="E66" s="311"/>
+      <c r="F66" s="311"/>
+      <c r="G66" s="311"/>
+      <c r="H66" s="311"/>
       <c r="I66" s="39">
         <f>'LKE ZI'!L206</f>
         <v>40</v>
@@ -7746,15 +7746,15 @@
       <c r="A68">
         <v>223</v>
       </c>
-      <c r="B68" s="304" t="s">
+      <c r="B68" s="308" t="s">
         <v>24</v>
       </c>
-      <c r="C68" s="305"/>
-      <c r="D68" s="305"/>
-      <c r="E68" s="305"/>
-      <c r="F68" s="305"/>
-      <c r="G68" s="305"/>
-      <c r="H68" s="305"/>
+      <c r="C68" s="309"/>
+      <c r="D68" s="309"/>
+      <c r="E68" s="309"/>
+      <c r="F68" s="309"/>
+      <c r="G68" s="309"/>
+      <c r="H68" s="309"/>
       <c r="I68" s="11">
         <f>'LKE ZI'!L208</f>
         <v>95.576190476190476</v>
@@ -7804,12 +7804,53 @@
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0"/>
   <mergeCells count="65">
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="B66:H66"/>
+    <mergeCell ref="B68:H68"/>
+    <mergeCell ref="D64:G64"/>
+    <mergeCell ref="E62:G62"/>
+    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="B58:H58"/>
+    <mergeCell ref="C60:G60"/>
+    <mergeCell ref="D61:G61"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="D34:G34"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="F25:G25"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="F9:G9"/>
@@ -7822,53 +7863,12 @@
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="D34:G34"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="B58:H58"/>
-    <mergeCell ref="C60:G60"/>
-    <mergeCell ref="D61:G61"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="F56:G56"/>
-    <mergeCell ref="B66:H66"/>
-    <mergeCell ref="B68:H68"/>
-    <mergeCell ref="D64:G64"/>
-    <mergeCell ref="E62:G62"/>
-    <mergeCell ref="E63:G63"/>
-    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="F6:G6"/>
   </mergeCells>
   <pageMargins left="2.3622047244094491" right="0.9055118110236221" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="5" scale="60" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -7882,8 +7882,8 @@
   </sheetPr>
   <dimension ref="A1:Q222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B169" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="G172" sqref="G172"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75"/>
@@ -7909,36 +7909,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="99.6" customHeight="1">
-      <c r="B1" s="335" t="s">
+      <c r="B1" s="314" t="s">
         <v>366</v>
       </c>
-      <c r="C1" s="336"/>
-      <c r="D1" s="336"/>
-      <c r="E1" s="336"/>
-      <c r="F1" s="336"/>
-      <c r="G1" s="336"/>
-      <c r="H1" s="336"/>
-      <c r="I1" s="336"/>
-      <c r="J1" s="336"/>
-      <c r="K1" s="336"/>
-      <c r="L1" s="336"/>
-      <c r="M1" s="336"/>
-      <c r="N1" s="336"/>
-      <c r="O1" s="336"/>
+      <c r="C1" s="315"/>
+      <c r="D1" s="315"/>
+      <c r="E1" s="315"/>
+      <c r="F1" s="315"/>
+      <c r="G1" s="315"/>
+      <c r="H1" s="315"/>
+      <c r="I1" s="315"/>
+      <c r="J1" s="315"/>
+      <c r="K1" s="315"/>
+      <c r="L1" s="315"/>
+      <c r="M1" s="315"/>
+      <c r="N1" s="315"/>
+      <c r="O1" s="315"/>
       <c r="P1" s="268"/>
     </row>
     <row r="2" spans="1:17" s="73" customFormat="1" ht="40.5">
       <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2" s="333" t="s">
+      <c r="B2" s="317" t="s">
         <v>106</v>
       </c>
-      <c r="C2" s="333"/>
-      <c r="D2" s="333"/>
-      <c r="E2" s="333"/>
-      <c r="F2" s="333"/>
-      <c r="G2" s="333"/>
+      <c r="C2" s="317"/>
+      <c r="D2" s="317"/>
+      <c r="E2" s="317"/>
+      <c r="F2" s="317"/>
+      <c r="G2" s="317"/>
       <c r="H2" s="113" t="s">
         <v>107</v>
       </c>
@@ -7990,13 +7990,13 @@
       <c r="B4" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="334" t="s">
+      <c r="C4" s="318" t="s">
         <v>105</v>
       </c>
-      <c r="D4" s="334"/>
-      <c r="E4" s="334"/>
-      <c r="F4" s="334"/>
-      <c r="G4" s="334"/>
+      <c r="D4" s="318"/>
+      <c r="E4" s="318"/>
+      <c r="F4" s="318"/>
+      <c r="G4" s="318"/>
       <c r="H4" s="84">
         <v>60</v>
       </c>
@@ -8022,12 +8022,12 @@
       <c r="C5" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="331" t="s">
+      <c r="D5" s="319" t="s">
         <v>110</v>
       </c>
-      <c r="E5" s="331"/>
-      <c r="F5" s="331"/>
-      <c r="G5" s="331"/>
+      <c r="E5" s="319"/>
+      <c r="F5" s="319"/>
+      <c r="G5" s="319"/>
       <c r="H5" s="90">
         <v>30</v>
       </c>
@@ -8054,11 +8054,11 @@
       <c r="D6" s="96" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="330" t="s">
+      <c r="E6" s="316" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="330"/>
-      <c r="G6" s="330"/>
+      <c r="F6" s="316"/>
+      <c r="G6" s="316"/>
       <c r="H6" s="97">
         <v>4</v>
       </c>
@@ -8086,10 +8086,10 @@
       <c r="E7" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="F7" s="330" t="s">
+      <c r="F7" s="316" t="s">
         <v>331</v>
       </c>
-      <c r="G7" s="330"/>
+      <c r="G7" s="316"/>
       <c r="H7" s="103">
         <v>0.5</v>
       </c>
@@ -8195,10 +8195,10 @@
       <c r="E10" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="F10" s="330" t="s">
+      <c r="F10" s="316" t="s">
         <v>59</v>
       </c>
-      <c r="G10" s="330"/>
+      <c r="G10" s="316"/>
       <c r="H10" s="103">
         <v>1</v>
       </c>
@@ -8343,10 +8343,10 @@
       <c r="E14" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="F14" s="330" t="s">
+      <c r="F14" s="316" t="s">
         <v>60</v>
       </c>
-      <c r="G14" s="330"/>
+      <c r="G14" s="316"/>
       <c r="H14" s="103">
         <v>1</v>
       </c>
@@ -8493,10 +8493,10 @@
       <c r="E18" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="F18" s="330" t="s">
+      <c r="F18" s="316" t="s">
         <v>61</v>
       </c>
-      <c r="G18" s="330"/>
+      <c r="G18" s="316"/>
       <c r="H18" s="103">
         <v>1.5</v>
       </c>
@@ -8679,11 +8679,11 @@
       <c r="D23" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="E23" s="330" t="s">
+      <c r="E23" s="316" t="s">
         <v>45</v>
       </c>
-      <c r="F23" s="330"/>
-      <c r="G23" s="330"/>
+      <c r="F23" s="316"/>
+      <c r="G23" s="316"/>
       <c r="H23" s="97">
         <v>3.5</v>
       </c>
@@ -8711,10 +8711,10 @@
       <c r="E24" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="F24" s="330" t="s">
+      <c r="F24" s="316" t="s">
         <v>212</v>
       </c>
-      <c r="G24" s="330"/>
+      <c r="G24" s="316"/>
       <c r="H24" s="103">
         <v>1</v>
       </c>
@@ -8861,10 +8861,10 @@
       <c r="E28" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="F28" s="330" t="s">
+      <c r="F28" s="316" t="s">
         <v>216</v>
       </c>
-      <c r="G28" s="330"/>
+      <c r="G28" s="316"/>
       <c r="H28" s="103">
         <v>2</v>
       </c>
@@ -9050,10 +9050,10 @@
       <c r="E33" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="F33" s="330" t="s">
+      <c r="F33" s="316" t="s">
         <v>62</v>
       </c>
-      <c r="G33" s="330"/>
+      <c r="G33" s="316"/>
       <c r="H33" s="103">
         <v>0.5</v>
       </c>
@@ -9159,11 +9159,11 @@
       <c r="D36" s="96" t="s">
         <v>113</v>
       </c>
-      <c r="E36" s="330" t="s">
+      <c r="E36" s="316" t="s">
         <v>134</v>
       </c>
-      <c r="F36" s="330"/>
-      <c r="G36" s="330"/>
+      <c r="F36" s="316"/>
+      <c r="G36" s="316"/>
       <c r="H36" s="97">
         <v>5</v>
       </c>
@@ -9192,10 +9192,10 @@
       <c r="E37" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="F37" s="330" t="s">
+      <c r="F37" s="316" t="s">
         <v>219</v>
       </c>
-      <c r="G37" s="330"/>
+      <c r="G37" s="316"/>
       <c r="H37" s="103">
         <v>0.25</v>
       </c>
@@ -9341,10 +9341,10 @@
       <c r="E41" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="F41" s="330" t="s">
+      <c r="F41" s="316" t="s">
         <v>63</v>
       </c>
-      <c r="G41" s="330"/>
+      <c r="G41" s="316"/>
       <c r="H41" s="103">
         <v>0.5</v>
       </c>
@@ -9492,10 +9492,10 @@
       <c r="E45" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="F45" s="330" t="s">
+      <c r="F45" s="316" t="s">
         <v>220</v>
       </c>
-      <c r="G45" s="330"/>
+      <c r="G45" s="316"/>
       <c r="H45" s="103">
         <v>1.25</v>
       </c>
@@ -9760,10 +9760,10 @@
       <c r="E52" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="F52" s="330" t="s">
+      <c r="F52" s="316" t="s">
         <v>221</v>
       </c>
-      <c r="G52" s="330"/>
+      <c r="G52" s="316"/>
       <c r="H52" s="103">
         <v>2</v>
       </c>
@@ -9952,10 +9952,10 @@
       <c r="E57" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="F57" s="330" t="s">
+      <c r="F57" s="316" t="s">
         <v>222</v>
       </c>
-      <c r="G57" s="330"/>
+      <c r="G57" s="316"/>
       <c r="H57" s="103">
         <v>0.75</v>
       </c>
@@ -10023,10 +10023,10 @@
       <c r="E59" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="F59" s="330" t="s">
+      <c r="F59" s="316" t="s">
         <v>64</v>
       </c>
-      <c r="G59" s="330"/>
+      <c r="G59" s="316"/>
       <c r="H59" s="103">
         <v>0.25</v>
       </c>
@@ -10093,11 +10093,11 @@
       <c r="D61" s="96" t="s">
         <v>114</v>
       </c>
-      <c r="E61" s="330" t="s">
+      <c r="E61" s="316" t="s">
         <v>48</v>
       </c>
-      <c r="F61" s="330"/>
-      <c r="G61" s="330"/>
+      <c r="F61" s="316"/>
+      <c r="G61" s="316"/>
       <c r="H61" s="97">
         <v>5</v>
       </c>
@@ -10126,10 +10126,10 @@
       <c r="E62" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="F62" s="330" t="s">
+      <c r="F62" s="316" t="s">
         <v>223</v>
       </c>
-      <c r="G62" s="330"/>
+      <c r="G62" s="316"/>
       <c r="H62" s="103">
         <v>2.5</v>
       </c>
@@ -10277,10 +10277,10 @@
       <c r="E66" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="F66" s="330" t="s">
+      <c r="F66" s="316" t="s">
         <v>65</v>
       </c>
-      <c r="G66" s="330"/>
+      <c r="G66" s="316"/>
       <c r="H66" s="103">
         <v>2.5</v>
       </c>
@@ -10620,11 +10620,11 @@
       <c r="D75" s="96" t="s">
         <v>17</v>
       </c>
-      <c r="E75" s="330" t="s">
+      <c r="E75" s="316" t="s">
         <v>49</v>
       </c>
-      <c r="F75" s="330"/>
-      <c r="G75" s="330"/>
+      <c r="F75" s="316"/>
+      <c r="G75" s="316"/>
       <c r="H75" s="97">
         <v>7.5</v>
       </c>
@@ -10653,10 +10653,10 @@
       <c r="E76" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="F76" s="330" t="s">
+      <c r="F76" s="316" t="s">
         <v>66</v>
       </c>
-      <c r="G76" s="330"/>
+      <c r="G76" s="316"/>
       <c r="H76" s="103">
         <v>1.5</v>
       </c>
@@ -10763,10 +10763,10 @@
       <c r="E79" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="F79" s="330" t="s">
+      <c r="F79" s="316" t="s">
         <v>270</v>
       </c>
-      <c r="G79" s="330"/>
+      <c r="G79" s="316"/>
       <c r="H79" s="103">
         <v>1.5</v>
       </c>
@@ -10953,10 +10953,10 @@
       <c r="E84" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="F84" s="330" t="s">
+      <c r="F84" s="316" t="s">
         <v>67</v>
       </c>
-      <c r="G84" s="330"/>
+      <c r="G84" s="316"/>
       <c r="H84" s="103">
         <v>1.5</v>
       </c>
@@ -11133,10 +11133,10 @@
       <c r="E89" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="F89" s="332" t="s">
+      <c r="F89" s="320" t="s">
         <v>68</v>
       </c>
-      <c r="G89" s="332"/>
+      <c r="G89" s="320"/>
       <c r="H89" s="103">
         <v>1.5</v>
       </c>
@@ -11299,10 +11299,10 @@
       <c r="E94" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="F94" s="330" t="s">
+      <c r="F94" s="316" t="s">
         <v>69</v>
       </c>
-      <c r="G94" s="330"/>
+      <c r="G94" s="316"/>
       <c r="H94" s="103">
         <v>1.5</v>
       </c>
@@ -11517,11 +11517,11 @@
       <c r="D100" s="96" t="s">
         <v>18</v>
       </c>
-      <c r="E100" s="330" t="s">
+      <c r="E100" s="316" t="s">
         <v>51</v>
       </c>
-      <c r="F100" s="330"/>
-      <c r="G100" s="330"/>
+      <c r="F100" s="316"/>
+      <c r="G100" s="316"/>
       <c r="H100" s="97">
         <v>5</v>
       </c>
@@ -11550,10 +11550,10 @@
       <c r="E101" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="F101" s="330" t="s">
+      <c r="F101" s="316" t="s">
         <v>70</v>
       </c>
-      <c r="G101" s="330"/>
+      <c r="G101" s="316"/>
       <c r="H101" s="103">
         <v>1</v>
       </c>
@@ -11730,10 +11730,10 @@
       <c r="E106" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="F106" s="330" t="s">
+      <c r="F106" s="316" t="s">
         <v>71</v>
       </c>
-      <c r="G106" s="330"/>
+      <c r="G106" s="316"/>
       <c r="H106" s="103">
         <v>1</v>
       </c>
@@ -11984,10 +11984,10 @@
       <c r="E113" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="F113" s="330" t="s">
+      <c r="F113" s="316" t="s">
         <v>316</v>
       </c>
-      <c r="G113" s="330"/>
+      <c r="G113" s="316"/>
       <c r="H113" s="103">
         <v>1</v>
       </c>
@@ -12129,10 +12129,10 @@
       <c r="E117" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="F117" s="330" t="s">
+      <c r="F117" s="316" t="s">
         <v>293</v>
       </c>
-      <c r="G117" s="330"/>
+      <c r="G117" s="316"/>
       <c r="H117" s="103">
         <v>1</v>
       </c>
@@ -12270,10 +12270,10 @@
       <c r="E121" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="F121" s="330" t="s">
+      <c r="F121" s="316" t="s">
         <v>321</v>
       </c>
-      <c r="G121" s="330"/>
+      <c r="G121" s="316"/>
       <c r="H121" s="103">
         <v>1</v>
       </c>
@@ -12407,12 +12407,12 @@
       <c r="C125" s="89" t="s">
         <v>12</v>
       </c>
-      <c r="D125" s="331" t="s">
+      <c r="D125" s="319" t="s">
         <v>75</v>
       </c>
-      <c r="E125" s="331"/>
-      <c r="F125" s="331"/>
-      <c r="G125" s="331"/>
+      <c r="E125" s="319"/>
+      <c r="F125" s="319"/>
+      <c r="G125" s="319"/>
       <c r="H125" s="90">
         <v>30</v>
       </c>
@@ -12440,11 +12440,11 @@
       <c r="D126" s="96" t="s">
         <v>14</v>
       </c>
-      <c r="E126" s="330" t="s">
+      <c r="E126" s="316" t="s">
         <v>43</v>
       </c>
-      <c r="F126" s="330"/>
-      <c r="G126" s="330"/>
+      <c r="F126" s="316"/>
+      <c r="G126" s="316"/>
       <c r="H126" s="97">
         <v>4</v>
       </c>
@@ -12473,10 +12473,10 @@
       <c r="E127" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="F127" s="330" t="s">
+      <c r="F127" s="316" t="s">
         <v>76</v>
       </c>
-      <c r="G127" s="330"/>
+      <c r="G127" s="316"/>
       <c r="H127" s="103">
         <v>2</v>
       </c>
@@ -12701,10 +12701,10 @@
       <c r="E134" s="130" t="s">
         <v>115</v>
       </c>
-      <c r="F134" s="325" t="s">
+      <c r="F134" s="321" t="s">
         <v>77</v>
       </c>
-      <c r="G134" s="325" t="s">
+      <c r="G134" s="321" t="s">
         <v>77</v>
       </c>
       <c r="H134" s="144">
@@ -12772,10 +12772,10 @@
       <c r="E136" s="130" t="s">
         <v>116</v>
       </c>
-      <c r="F136" s="325" t="s">
+      <c r="F136" s="321" t="s">
         <v>79</v>
       </c>
-      <c r="G136" s="325" t="s">
+      <c r="G136" s="321" t="s">
         <v>79</v>
       </c>
       <c r="H136" s="144">
@@ -12842,11 +12842,11 @@
       <c r="D138" s="154" t="s">
         <v>15</v>
       </c>
-      <c r="E138" s="325" t="s">
+      <c r="E138" s="321" t="s">
         <v>45</v>
       </c>
-      <c r="F138" s="325"/>
-      <c r="G138" s="325"/>
+      <c r="F138" s="321"/>
+      <c r="G138" s="321"/>
       <c r="H138" s="155">
         <v>3.5</v>
       </c>
@@ -12876,10 +12876,10 @@
       <c r="E139" s="130" t="s">
         <v>111</v>
       </c>
-      <c r="F139" s="325" t="s">
+      <c r="F139" s="321" t="s">
         <v>83</v>
       </c>
-      <c r="G139" s="325"/>
+      <c r="G139" s="321"/>
       <c r="H139" s="144">
         <v>0.5</v>
       </c>
@@ -12945,10 +12945,10 @@
       <c r="E141" s="130" t="s">
         <v>115</v>
       </c>
-      <c r="F141" s="325" t="s">
+      <c r="F141" s="321" t="s">
         <v>84</v>
       </c>
-      <c r="G141" s="325"/>
+      <c r="G141" s="321"/>
       <c r="H141" s="144">
         <v>1</v>
       </c>
@@ -13050,10 +13050,10 @@
       <c r="E144" s="130" t="s">
         <v>116</v>
       </c>
-      <c r="F144" s="325" t="s">
+      <c r="F144" s="321" t="s">
         <v>89</v>
       </c>
-      <c r="G144" s="325"/>
+      <c r="G144" s="321"/>
       <c r="H144" s="144">
         <v>2</v>
       </c>
@@ -13190,11 +13190,11 @@
       <c r="D148" s="154" t="s">
         <v>113</v>
       </c>
-      <c r="E148" s="325" t="s">
+      <c r="E148" s="321" t="s">
         <v>134</v>
       </c>
-      <c r="F148" s="325"/>
-      <c r="G148" s="325"/>
+      <c r="F148" s="321"/>
+      <c r="G148" s="321"/>
       <c r="H148" s="155">
         <v>5</v>
       </c>
@@ -13224,10 +13224,10 @@
       <c r="E149" s="130" t="s">
         <v>111</v>
       </c>
-      <c r="F149" s="325" t="s">
+      <c r="F149" s="321" t="s">
         <v>93</v>
       </c>
-      <c r="G149" s="325"/>
+      <c r="G149" s="321"/>
       <c r="H149" s="144">
         <v>1.5</v>
       </c>
@@ -13293,10 +13293,10 @@
       <c r="E151" s="130" t="s">
         <v>115</v>
       </c>
-      <c r="F151" s="325" t="s">
+      <c r="F151" s="321" t="s">
         <v>121</v>
       </c>
-      <c r="G151" s="325"/>
+      <c r="G151" s="321"/>
       <c r="H151" s="144">
         <v>1.5</v>
       </c>
@@ -13362,10 +13362,10 @@
       <c r="E153" s="130" t="s">
         <v>116</v>
       </c>
-      <c r="F153" s="325" t="s">
+      <c r="F153" s="321" t="s">
         <v>94</v>
       </c>
-      <c r="G153" s="325"/>
+      <c r="G153" s="321"/>
       <c r="H153" s="144">
         <v>2</v>
       </c>
@@ -13525,11 +13525,11 @@
       <c r="D158" s="154" t="s">
         <v>114</v>
       </c>
-      <c r="E158" s="325" t="s">
+      <c r="E158" s="321" t="s">
         <v>48</v>
       </c>
-      <c r="F158" s="325"/>
-      <c r="G158" s="325"/>
+      <c r="F158" s="321"/>
+      <c r="G158" s="321"/>
       <c r="H158" s="155">
         <v>5</v>
       </c>
@@ -13556,10 +13556,10 @@
       <c r="E159" s="130" t="s">
         <v>111</v>
       </c>
-      <c r="F159" s="325" t="s">
+      <c r="F159" s="321" t="s">
         <v>136</v>
       </c>
-      <c r="G159" s="325"/>
+      <c r="G159" s="321"/>
       <c r="H159" s="144">
         <v>2</v>
       </c>
@@ -13688,10 +13688,10 @@
       <c r="E163" s="130" t="s">
         <v>115</v>
       </c>
-      <c r="F163" s="325" t="s">
+      <c r="F163" s="321" t="s">
         <v>298</v>
       </c>
-      <c r="G163" s="325"/>
+      <c r="G163" s="321"/>
       <c r="H163" s="144">
         <v>1.5</v>
       </c>
@@ -13757,10 +13757,10 @@
       <c r="E165" s="130" t="s">
         <v>116</v>
       </c>
-      <c r="F165" s="325" t="s">
+      <c r="F165" s="321" t="s">
         <v>97</v>
       </c>
-      <c r="G165" s="325"/>
+      <c r="G165" s="321"/>
       <c r="H165" s="144">
         <v>1.5</v>
       </c>
@@ -13825,11 +13825,11 @@
       <c r="D167" s="154" t="s">
         <v>17</v>
       </c>
-      <c r="E167" s="325" t="s">
+      <c r="E167" s="321" t="s">
         <v>49</v>
       </c>
-      <c r="F167" s="325"/>
-      <c r="G167" s="325"/>
+      <c r="F167" s="321"/>
+      <c r="G167" s="321"/>
       <c r="H167" s="155">
         <v>7.5</v>
       </c>
@@ -13859,10 +13859,10 @@
       <c r="E168" s="143" t="s">
         <v>111</v>
       </c>
-      <c r="F168" s="325" t="s">
+      <c r="F168" s="321" t="s">
         <v>326</v>
       </c>
-      <c r="G168" s="325"/>
+      <c r="G168" s="321"/>
       <c r="H168" s="144">
         <v>2.5</v>
       </c>
@@ -13926,10 +13926,10 @@
       <c r="E170" s="143" t="s">
         <v>115</v>
       </c>
-      <c r="F170" s="325" t="s">
+      <c r="F170" s="321" t="s">
         <v>28</v>
       </c>
-      <c r="G170" s="325"/>
+      <c r="G170" s="321"/>
       <c r="H170" s="144">
         <v>3</v>
       </c>
@@ -14090,10 +14090,10 @@
       <c r="E175" s="143" t="s">
         <v>116</v>
       </c>
-      <c r="F175" s="325" t="s">
+      <c r="F175" s="321" t="s">
         <v>355</v>
       </c>
-      <c r="G175" s="325"/>
+      <c r="G175" s="321"/>
       <c r="H175" s="144">
         <v>2</v>
       </c>
@@ -14125,10 +14125,10 @@
       <c r="E176" s="171" t="s">
         <v>111</v>
       </c>
-      <c r="F176" s="328" t="s">
+      <c r="F176" s="324" t="s">
         <v>341</v>
       </c>
-      <c r="G176" s="329"/>
+      <c r="G176" s="325"/>
       <c r="H176" s="172">
         <v>1</v>
       </c>
@@ -14351,10 +14351,10 @@
       <c r="C183" s="171"/>
       <c r="D183" s="171"/>
       <c r="E183" s="171"/>
-      <c r="F183" s="326" t="s">
+      <c r="F183" s="322" t="s">
         <v>98</v>
       </c>
-      <c r="G183" s="327"/>
+      <c r="G183" s="323"/>
       <c r="H183" s="181">
         <v>1</v>
       </c>
@@ -14577,11 +14577,11 @@
       <c r="D190" s="154" t="s">
         <v>18</v>
       </c>
-      <c r="E190" s="325" t="s">
+      <c r="E190" s="321" t="s">
         <v>51</v>
       </c>
-      <c r="F190" s="325"/>
-      <c r="G190" s="325"/>
+      <c r="F190" s="321"/>
+      <c r="G190" s="321"/>
       <c r="H190" s="155">
         <v>5</v>
       </c>
@@ -14611,10 +14611,10 @@
       <c r="E191" s="194" t="s">
         <v>111</v>
       </c>
-      <c r="F191" s="325" t="s">
+      <c r="F191" s="321" t="s">
         <v>102</v>
       </c>
-      <c r="G191" s="325"/>
+      <c r="G191" s="321"/>
       <c r="H191" s="144">
         <v>2.5</v>
       </c>
@@ -14775,10 +14775,10 @@
       <c r="E196" s="194" t="s">
         <v>115</v>
       </c>
-      <c r="F196" s="316" t="s">
+      <c r="F196" s="333" t="s">
         <v>103</v>
       </c>
-      <c r="G196" s="317"/>
+      <c r="G196" s="334"/>
       <c r="H196" s="144">
         <v>2.5</v>
       </c>
@@ -14838,16 +14838,16 @@
       <c r="A198">
         <v>211</v>
       </c>
-      <c r="B198" s="318" t="s">
+      <c r="B198" s="335" t="s">
         <v>127</v>
       </c>
-      <c r="C198" s="318"/>
-      <c r="D198" s="318"/>
-      <c r="E198" s="318"/>
-      <c r="F198" s="318"/>
-      <c r="G198" s="318"/>
-      <c r="H198" s="318"/>
-      <c r="I198" s="318"/>
+      <c r="C198" s="335"/>
+      <c r="D198" s="335"/>
+      <c r="E198" s="335"/>
+      <c r="F198" s="335"/>
+      <c r="G198" s="335"/>
+      <c r="H198" s="335"/>
+      <c r="I198" s="335"/>
       <c r="J198" s="197"/>
       <c r="K198" s="197"/>
       <c r="L198" s="197">
@@ -14888,13 +14888,13 @@
       <c r="B200" s="207" t="s">
         <v>13</v>
       </c>
-      <c r="C200" s="319" t="s">
+      <c r="C200" s="336" t="s">
         <v>128</v>
       </c>
-      <c r="D200" s="319"/>
-      <c r="E200" s="319"/>
-      <c r="F200" s="319"/>
-      <c r="G200" s="319"/>
+      <c r="D200" s="336"/>
+      <c r="E200" s="336"/>
+      <c r="F200" s="336"/>
+      <c r="G200" s="336"/>
       <c r="H200" s="208">
         <v>40</v>
       </c>
@@ -14922,12 +14922,12 @@
       <c r="C201" s="210" t="s">
         <v>1</v>
       </c>
-      <c r="D201" s="314" t="s">
+      <c r="D201" s="331" t="s">
         <v>300</v>
       </c>
-      <c r="E201" s="314"/>
-      <c r="F201" s="314"/>
-      <c r="G201" s="314"/>
+      <c r="E201" s="331"/>
+      <c r="F201" s="331"/>
+      <c r="G201" s="331"/>
       <c r="H201" s="208">
         <v>22.5</v>
       </c>
@@ -14956,11 +14956,11 @@
       <c r="D202" s="217" t="s">
         <v>41</v>
       </c>
-      <c r="E202" s="315" t="s">
+      <c r="E202" s="332" t="s">
         <v>129</v>
       </c>
-      <c r="F202" s="315"/>
-      <c r="G202" s="315"/>
+      <c r="F202" s="332"/>
+      <c r="G202" s="332"/>
       <c r="H202" s="218">
         <v>17.5</v>
       </c>
@@ -14994,11 +14994,11 @@
       <c r="D203" s="217" t="s">
         <v>42</v>
       </c>
-      <c r="E203" s="315" t="s">
+      <c r="E203" s="332" t="s">
         <v>199</v>
       </c>
-      <c r="F203" s="315"/>
-      <c r="G203" s="315"/>
+      <c r="F203" s="332"/>
+      <c r="G203" s="332"/>
       <c r="H203" s="218">
         <v>5</v>
       </c>
@@ -15031,12 +15031,12 @@
       <c r="C204" s="210" t="s">
         <v>12</v>
       </c>
-      <c r="D204" s="314" t="s">
+      <c r="D204" s="331" t="s">
         <v>301</v>
       </c>
-      <c r="E204" s="314"/>
-      <c r="F204" s="314"/>
-      <c r="G204" s="314"/>
+      <c r="E204" s="331"/>
+      <c r="F204" s="331"/>
+      <c r="G204" s="331"/>
       <c r="H204" s="208">
         <v>17.5</v>
       </c>
@@ -15065,11 +15065,11 @@
       <c r="D205" s="226" t="s">
         <v>41</v>
       </c>
-      <c r="E205" s="321" t="s">
+      <c r="E205" s="327" t="s">
         <v>130</v>
       </c>
-      <c r="F205" s="321"/>
-      <c r="G205" s="321"/>
+      <c r="F205" s="327"/>
+      <c r="G205" s="327"/>
       <c r="H205" s="227">
         <v>17.5</v>
       </c>
@@ -15098,16 +15098,16 @@
       <c r="A206">
         <v>221</v>
       </c>
-      <c r="B206" s="322" t="s">
+      <c r="B206" s="328" t="s">
         <v>23</v>
       </c>
-      <c r="C206" s="322"/>
-      <c r="D206" s="322"/>
-      <c r="E206" s="322"/>
-      <c r="F206" s="322"/>
-      <c r="G206" s="322"/>
-      <c r="H206" s="322"/>
-      <c r="I206" s="322"/>
+      <c r="C206" s="328"/>
+      <c r="D206" s="328"/>
+      <c r="E206" s="328"/>
+      <c r="F206" s="328"/>
+      <c r="G206" s="328"/>
+      <c r="H206" s="328"/>
+      <c r="I206" s="328"/>
       <c r="J206" s="197"/>
       <c r="K206" s="197"/>
       <c r="L206" s="197">
@@ -15145,18 +15145,18 @@
       <c r="A208" s="117">
         <v>223</v>
       </c>
-      <c r="B208" s="323" t="s">
+      <c r="B208" s="329" t="s">
         <v>364</v>
       </c>
-      <c r="C208" s="323"/>
-      <c r="D208" s="323"/>
-      <c r="E208" s="323"/>
-      <c r="F208" s="323"/>
-      <c r="G208" s="323"/>
-      <c r="H208" s="323"/>
-      <c r="I208" s="323"/>
-      <c r="J208" s="323"/>
-      <c r="K208" s="323"/>
+      <c r="C208" s="329"/>
+      <c r="D208" s="329"/>
+      <c r="E208" s="329"/>
+      <c r="F208" s="329"/>
+      <c r="G208" s="329"/>
+      <c r="H208" s="329"/>
+      <c r="I208" s="329"/>
+      <c r="J208" s="329"/>
+      <c r="K208" s="329"/>
       <c r="L208" s="232">
         <f>SUM(L198,L206)</f>
         <v>95.576190476190476</v>
@@ -15248,13 +15248,13 @@
       <c r="G213" s="239"/>
       <c r="H213" s="240"/>
       <c r="I213" s="241"/>
-      <c r="J213" s="324" t="s">
+      <c r="J213" s="330" t="s">
         <v>365</v>
       </c>
-      <c r="K213" s="324"/>
-      <c r="L213" s="324"/>
-      <c r="M213" s="324"/>
-      <c r="N213" s="324"/>
+      <c r="K213" s="330"/>
+      <c r="L213" s="330"/>
+      <c r="M213" s="330"/>
+      <c r="N213" s="330"/>
       <c r="O213" s="251"/>
       <c r="P213" s="302"/>
       <c r="Q213" s="138"/>
@@ -15268,11 +15268,11 @@
       <c r="G214" s="239"/>
       <c r="H214" s="240"/>
       <c r="I214" s="241"/>
-      <c r="J214" s="324"/>
-      <c r="K214" s="324"/>
-      <c r="L214" s="324"/>
-      <c r="M214" s="324"/>
-      <c r="N214" s="324"/>
+      <c r="J214" s="330"/>
+      <c r="K214" s="330"/>
+      <c r="L214" s="330"/>
+      <c r="M214" s="330"/>
+      <c r="N214" s="330"/>
       <c r="O214" s="251"/>
       <c r="P214" s="302"/>
       <c r="Q214" s="138"/>
@@ -15286,11 +15286,11 @@
       <c r="G215" s="239"/>
       <c r="H215" s="240"/>
       <c r="I215" s="241"/>
-      <c r="J215" s="324"/>
-      <c r="K215" s="324"/>
-      <c r="L215" s="324"/>
-      <c r="M215" s="324"/>
-      <c r="N215" s="324"/>
+      <c r="J215" s="330"/>
+      <c r="K215" s="330"/>
+      <c r="L215" s="330"/>
+      <c r="M215" s="330"/>
+      <c r="N215" s="330"/>
       <c r="O215" s="251"/>
       <c r="P215" s="302"/>
       <c r="Q215" s="138"/>
@@ -15304,11 +15304,11 @@
       <c r="G216" s="239"/>
       <c r="H216" s="240"/>
       <c r="I216" s="241"/>
-      <c r="J216" s="324"/>
-      <c r="K216" s="324"/>
-      <c r="L216" s="324"/>
-      <c r="M216" s="324"/>
-      <c r="N216" s="324"/>
+      <c r="J216" s="330"/>
+      <c r="K216" s="330"/>
+      <c r="L216" s="330"/>
+      <c r="M216" s="330"/>
+      <c r="N216" s="330"/>
       <c r="O216" s="251"/>
       <c r="P216" s="302"/>
       <c r="Q216" s="244"/>
@@ -15322,11 +15322,11 @@
       <c r="G217" s="239"/>
       <c r="H217" s="240"/>
       <c r="I217" s="241"/>
-      <c r="J217" s="324"/>
-      <c r="K217" s="324"/>
-      <c r="L217" s="324"/>
-      <c r="M217" s="324"/>
-      <c r="N217" s="324"/>
+      <c r="J217" s="330"/>
+      <c r="K217" s="330"/>
+      <c r="L217" s="330"/>
+      <c r="M217" s="330"/>
+      <c r="N217" s="330"/>
       <c r="O217" s="251"/>
       <c r="P217" s="302"/>
       <c r="Q217" s="244"/>
@@ -15414,11 +15414,11 @@
       <c r="G222" s="239"/>
       <c r="H222" s="240"/>
       <c r="I222" s="241"/>
-      <c r="J222" s="320" t="s">
+      <c r="J222" s="326" t="s">
         <v>330</v>
       </c>
-      <c r="K222" s="320"/>
-      <c r="L222" s="320"/>
+      <c r="K222" s="326"/>
+      <c r="L222" s="326"/>
       <c r="M222" s="246"/>
       <c r="N222" s="244"/>
       <c r="O222" s="251"/>
@@ -15429,6 +15429,62 @@
   <sheetProtection formatColumns="0" formatRows="0" autoFilter="0"/>
   <autoFilter ref="A3:O208" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <mergeCells count="72">
+    <mergeCell ref="D201:G201"/>
+    <mergeCell ref="D204:G204"/>
+    <mergeCell ref="E202:G202"/>
+    <mergeCell ref="E203:G203"/>
+    <mergeCell ref="F196:G196"/>
+    <mergeCell ref="B198:I198"/>
+    <mergeCell ref="C200:G200"/>
+    <mergeCell ref="J222:L222"/>
+    <mergeCell ref="E205:G205"/>
+    <mergeCell ref="B206:I206"/>
+    <mergeCell ref="B208:K208"/>
+    <mergeCell ref="J213:N217"/>
+    <mergeCell ref="E167:G167"/>
+    <mergeCell ref="F191:G191"/>
+    <mergeCell ref="E190:G190"/>
+    <mergeCell ref="F159:G159"/>
+    <mergeCell ref="F163:G163"/>
+    <mergeCell ref="F165:G165"/>
+    <mergeCell ref="F168:G168"/>
+    <mergeCell ref="F170:G170"/>
+    <mergeCell ref="F183:G183"/>
+    <mergeCell ref="F176:G176"/>
+    <mergeCell ref="F175:G175"/>
+    <mergeCell ref="F144:G144"/>
+    <mergeCell ref="E148:G148"/>
+    <mergeCell ref="F149:G149"/>
+    <mergeCell ref="E158:G158"/>
+    <mergeCell ref="F151:G151"/>
+    <mergeCell ref="F153:G153"/>
+    <mergeCell ref="F134:G134"/>
+    <mergeCell ref="F136:G136"/>
+    <mergeCell ref="E138:G138"/>
+    <mergeCell ref="F139:G139"/>
+    <mergeCell ref="F141:G141"/>
+    <mergeCell ref="E75:G75"/>
+    <mergeCell ref="E100:G100"/>
+    <mergeCell ref="D125:G125"/>
+    <mergeCell ref="E126:G126"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="E61:G61"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="F79:G79"/>
+    <mergeCell ref="F84:G84"/>
+    <mergeCell ref="F89:G89"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="D5:G5"/>
     <mergeCell ref="B1:O1"/>
     <mergeCell ref="F94:G94"/>
     <mergeCell ref="F106:G106"/>
@@ -15445,62 +15501,6 @@
     <mergeCell ref="E36:G36"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="E75:G75"/>
-    <mergeCell ref="E100:G100"/>
-    <mergeCell ref="D125:G125"/>
-    <mergeCell ref="E126:G126"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="E61:G61"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="F79:G79"/>
-    <mergeCell ref="F84:G84"/>
-    <mergeCell ref="F89:G89"/>
-    <mergeCell ref="F134:G134"/>
-    <mergeCell ref="F136:G136"/>
-    <mergeCell ref="E138:G138"/>
-    <mergeCell ref="F139:G139"/>
-    <mergeCell ref="F141:G141"/>
-    <mergeCell ref="F144:G144"/>
-    <mergeCell ref="E148:G148"/>
-    <mergeCell ref="F149:G149"/>
-    <mergeCell ref="E158:G158"/>
-    <mergeCell ref="F151:G151"/>
-    <mergeCell ref="F153:G153"/>
-    <mergeCell ref="E167:G167"/>
-    <mergeCell ref="F191:G191"/>
-    <mergeCell ref="E190:G190"/>
-    <mergeCell ref="F159:G159"/>
-    <mergeCell ref="F163:G163"/>
-    <mergeCell ref="F165:G165"/>
-    <mergeCell ref="F168:G168"/>
-    <mergeCell ref="F170:G170"/>
-    <mergeCell ref="F183:G183"/>
-    <mergeCell ref="F176:G176"/>
-    <mergeCell ref="F175:G175"/>
-    <mergeCell ref="J222:L222"/>
-    <mergeCell ref="E205:G205"/>
-    <mergeCell ref="B206:I206"/>
-    <mergeCell ref="B208:K208"/>
-    <mergeCell ref="J213:N217"/>
-    <mergeCell ref="D201:G201"/>
-    <mergeCell ref="D204:G204"/>
-    <mergeCell ref="E202:G202"/>
-    <mergeCell ref="E203:G203"/>
-    <mergeCell ref="F196:G196"/>
-    <mergeCell ref="B198:I198"/>
-    <mergeCell ref="C200:G200"/>
   </mergeCells>
   <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K150 K12:K13 K29:K32 K63:K64 K51 K74 K60 K152 K34:K35 K77 K72 K82:K83 K124 K91:K93 K98:K99 K9 K20:K21 K115:K116 K142:K143 K119 K85 K87:K88" xr:uid="{00000000-0002-0000-0200-000000000000}">

</xml_diff>